<commit_message>
Updating fire regime weighting code to include all western species (including missing spp e.g. Larix occidentalis), and drop Tsuga outliers from Bark Thickness trait DB. Running overnight, hold off on pull requests until next commit.
</commit_message>
<xml_diff>
--- a/manuscript/tables/TableS1.xlsx
+++ b/manuscript/tables/TableS1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="240" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TableS1.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="40">
   <si>
     <t>Scientific_Name</t>
   </si>
@@ -204,7 +204,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -226,8 +226,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -240,17 +256,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -261,6 +274,14 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -271,6 +292,14 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -600,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:N31"/>
+      <selection sqref="A1:O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -614,16 +643,17 @@
     <col min="5" max="5" width="7" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" customWidth="1"/>
-    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="1.6640625" customWidth="1"/>
+    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1"/>
       <c r="B1" s="5" t="s">
         <v>32</v>
@@ -632,18 +662,19 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" ht="33" customHeight="1">
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" ht="33" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -665,29 +696,30 @@
       <c r="G2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -710,28 +742,31 @@
         <v>86.1</v>
       </c>
       <c r="H3" s="4">
-        <v>0.93103448300000002</v>
+        <v>1</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
       </c>
       <c r="J3" s="4">
-        <v>0.76923076899999998</v>
+        <v>1</v>
       </c>
       <c r="K3" s="4">
-        <v>0.93333333299999999</v>
+        <v>0.76923076923076905</v>
       </c>
       <c r="L3" s="4">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="M3" s="4">
         <v>0.8</v>
       </c>
-      <c r="M3" s="4">
-        <v>0.86666666699999995</v>
-      </c>
       <c r="N3" s="4">
-        <v>0.89147286800000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>0.86666666666666603</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0.90551181102362199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -754,160 +789,172 @@
         <v>90</v>
       </c>
       <c r="H4" s="4">
-        <v>0.75862068999999999</v>
+        <v>0.81481481481481399</v>
       </c>
       <c r="I4" s="4">
-        <v>0.75862068999999999</v>
+        <v>0.81481481481481399</v>
       </c>
       <c r="J4" s="4">
+        <v>0.75862068965517204</v>
+      </c>
+      <c r="K4" s="4">
         <v>1</v>
       </c>
-      <c r="K4" s="4">
-        <v>0.86666666699999995</v>
-      </c>
       <c r="L4" s="4">
-        <v>0.86666666699999995</v>
+        <v>0.86666666666666603</v>
       </c>
       <c r="M4" s="4">
-        <v>0.93333333299999999</v>
+        <v>0.86666666666666603</v>
       </c>
       <c r="N4" s="4">
-        <v>0.85271317800000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0.86614173228346403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4">
-        <v>1.8288</v>
+        <v>1.6002000000000001</v>
       </c>
       <c r="C5" s="4">
-        <v>62.285713999999999</v>
+        <v>51.095238000000002</v>
       </c>
       <c r="D5" s="4">
         <v>10</v>
       </c>
-      <c r="E5" s="4">
-        <v>128.5</v>
-      </c>
-      <c r="F5" s="4">
-        <v>55.6</v>
-      </c>
-      <c r="G5" s="4">
-        <v>77.099999999999994</v>
+      <c r="E5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="H5" s="4">
-        <v>0.82758620699999996</v>
+        <v>0.77777777777777701</v>
       </c>
       <c r="I5" s="4">
-        <v>0.93103448300000002</v>
+        <v>0.77777777777777701</v>
       </c>
       <c r="J5" s="4">
+        <v>0.65517241379310298</v>
+      </c>
+      <c r="K5" s="4">
         <v>1</v>
       </c>
-      <c r="K5" s="4">
-        <v>0.33333333300000001</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0.66666666699999999</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0.66666666699999999</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0.79069767400000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="L5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0.80487804878048697</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4">
-        <v>1.6002000000000001</v>
+        <v>1.8288</v>
       </c>
       <c r="C6" s="4">
-        <v>41.229047999999999</v>
+        <v>62.285713999999999</v>
       </c>
       <c r="D6" s="4">
         <v>10</v>
       </c>
       <c r="E6" s="4">
-        <v>79.7</v>
+        <v>128.5</v>
       </c>
       <c r="F6" s="4">
-        <v>77</v>
+        <v>55.6</v>
       </c>
       <c r="G6" s="4">
-        <v>92</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="H6" s="4">
-        <v>0.72413793100000001</v>
+        <v>0.88888888888888795</v>
       </c>
       <c r="I6" s="4">
-        <v>0.44827586200000002</v>
+        <v>0.88888888888888795</v>
       </c>
       <c r="J6" s="4">
+        <v>0.93103448275862</v>
+      </c>
+      <c r="K6" s="4">
         <v>1</v>
       </c>
-      <c r="K6" s="4">
-        <v>0.8</v>
-      </c>
       <c r="L6" s="4">
-        <v>1</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="M6" s="4">
-        <v>1</v>
+        <v>0.66666666666666596</v>
       </c>
       <c r="N6" s="4">
-        <v>0.79069767400000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0.80314960629921195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4">
         <v>1.6002000000000001</v>
       </c>
       <c r="C7" s="4">
-        <v>51.095238000000002</v>
+        <v>41.229047999999999</v>
       </c>
       <c r="D7" s="4">
         <v>10</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>3</v>
+      <c r="E7" s="4">
+        <v>79.7</v>
+      </c>
+      <c r="F7" s="4">
+        <v>77</v>
+      </c>
+      <c r="G7" s="4">
+        <v>92</v>
       </c>
       <c r="H7" s="4">
-        <v>0.72413793100000001</v>
+        <v>0.77777777777777701</v>
       </c>
       <c r="I7" s="4">
-        <v>0.65517241400000004</v>
+        <v>0.77777777777777701</v>
       </c>
       <c r="J7" s="4">
+        <v>0.44827586206896503</v>
+      </c>
+      <c r="K7" s="4">
         <v>1</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>3</v>
+      <c r="L7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1</v>
       </c>
       <c r="N7" s="4">
-        <v>0.78571428600000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>1</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0.80314960629921195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -930,28 +977,31 @@
         <v>75.8</v>
       </c>
       <c r="H8" s="4">
-        <v>0.93103448300000002</v>
+        <v>1</v>
       </c>
       <c r="I8" s="4">
-        <v>0.96551724100000003</v>
+        <v>1</v>
       </c>
       <c r="J8" s="4">
-        <v>0.84615384599999999</v>
+        <v>0.96551724137931005</v>
       </c>
       <c r="K8" s="4">
-        <v>0.26666666700000002</v>
+        <v>0.84615384615384603</v>
       </c>
       <c r="L8" s="4">
-        <v>0.46666666699999998</v>
+        <v>0.266666666666666</v>
       </c>
       <c r="M8" s="4">
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="N8" s="4">
         <v>0.6</v>
       </c>
-      <c r="N8" s="4">
-        <v>0.751937984</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="O8" s="4">
+        <v>0.76377952755905498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -974,28 +1024,31 @@
         <v>82.78</v>
       </c>
       <c r="H9" s="4">
-        <v>0.34482758600000002</v>
+        <v>0.37037037037037002</v>
       </c>
       <c r="I9" s="4">
-        <v>0.89655172400000005</v>
+        <v>0.37037037037037002</v>
       </c>
       <c r="J9" s="4">
-        <v>0.80769230800000003</v>
+        <v>0.89655172413793105</v>
       </c>
       <c r="K9" s="4">
+        <v>0.80769230769230704</v>
+      </c>
+      <c r="L9" s="4">
         <v>0.6</v>
       </c>
-      <c r="L9" s="4">
-        <v>0.93333333299999999</v>
-      </c>
       <c r="M9" s="4">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="N9" s="4">
         <v>0.8</v>
       </c>
-      <c r="N9" s="4">
-        <v>0.71317829499999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9" s="4">
+        <v>0.72440944881889702</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1018,16 +1071,16 @@
         <v>3</v>
       </c>
       <c r="H10" s="4">
-        <v>0.79310344799999999</v>
+        <v>0.85185185185185097</v>
       </c>
       <c r="I10" s="4">
-        <v>0.55172413799999998</v>
+        <v>0.85185185185185097</v>
       </c>
       <c r="J10" s="4">
-        <v>0.76923076899999998</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>3</v>
+        <v>0.55172413793103403</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0.76923076923076905</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>3</v>
@@ -1035,11 +1088,14 @@
       <c r="M10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N10" s="4">
-        <v>0.70238095199999995</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="N10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0.71951219512195097</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1062,16 +1118,16 @@
         <v>3</v>
       </c>
       <c r="H11" s="4">
-        <v>0.482758621</v>
+        <v>0.51851851851851805</v>
       </c>
       <c r="I11" s="4">
-        <v>0.82758620699999996</v>
+        <v>0.51851851851851805</v>
       </c>
       <c r="J11" s="4">
-        <v>0.76923076899999998</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>3</v>
+        <v>0.82758620689655105</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.76923076923076905</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>3</v>
@@ -1079,22 +1135,25 @@
       <c r="M11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="4">
-        <v>0.69047619000000005</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="N11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0.707317073170731</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4">
-        <v>5.5880000000000001</v>
+        <v>2.0573999999999999</v>
       </c>
       <c r="C12" s="4">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D12" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>3</v>
@@ -1109,13 +1168,13 @@
         <v>1</v>
       </c>
       <c r="I12" s="4">
-        <v>0.24137931000000001</v>
+        <v>1</v>
       </c>
       <c r="J12" s="4">
-        <v>0.76923076899999998</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>3</v>
+        <v>0.62068965517241304</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0.34615384615384598</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>3</v>
@@ -1123,22 +1182,25 @@
       <c r="M12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N12" s="4">
-        <v>0.66666666699999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="N12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0.65853658536585302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B13" s="4">
-        <v>2.0573999999999999</v>
+        <v>1.1684000000000001</v>
       </c>
       <c r="C13" s="4">
-        <v>50</v>
+        <v>59.424999999999997</v>
       </c>
       <c r="D13" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>3</v>
@@ -1150,16 +1212,16 @@
         <v>3</v>
       </c>
       <c r="H13" s="4">
-        <v>0.93103448300000002</v>
+        <v>0.55555555555555503</v>
       </c>
       <c r="I13" s="4">
-        <v>0.62068965499999995</v>
+        <v>0.55555555555555503</v>
       </c>
       <c r="J13" s="4">
-        <v>0.34615384599999999</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>3</v>
+        <v>0.86206896551724099</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0.46153846153846101</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>3</v>
@@ -1167,319 +1229,343 @@
       <c r="M13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N13" s="4">
-        <v>0.64285714299999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="N13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0.63414634146341398</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B14" s="4">
-        <v>1.1684000000000001</v>
+        <v>1.6002000000000001</v>
       </c>
       <c r="C14" s="4">
-        <v>59.424999999999997</v>
+        <v>54.256194000000001</v>
       </c>
       <c r="D14" s="4">
-        <v>4</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="E14" s="4">
+        <v>105.8</v>
+      </c>
+      <c r="F14" s="4">
+        <v>26.2</v>
+      </c>
+      <c r="G14" s="4">
+        <v>26.6</v>
       </c>
       <c r="H14" s="4">
-        <v>0.517241379</v>
+        <v>0.77777777777777701</v>
       </c>
       <c r="I14" s="4">
-        <v>0.86206896600000005</v>
+        <v>0.77777777777777701</v>
       </c>
       <c r="J14" s="4">
-        <v>0.46153846199999998</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>3</v>
+        <v>0.79310344827586199</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0.2</v>
       </c>
       <c r="N14" s="4">
-        <v>0.61904761900000005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>0.2</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0.60629921259842501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B15" s="4">
-        <v>1.6002000000000001</v>
+        <v>1.1938</v>
       </c>
       <c r="C15" s="4">
-        <v>54.256194000000001</v>
+        <v>51.27</v>
       </c>
       <c r="D15" s="4">
         <v>5</v>
       </c>
       <c r="E15" s="4">
-        <v>105.8</v>
+        <v>79.8</v>
       </c>
       <c r="F15" s="4">
-        <v>26.2</v>
+        <v>38.4</v>
       </c>
       <c r="G15" s="4">
-        <v>26.6</v>
+        <v>32</v>
       </c>
       <c r="H15" s="4">
-        <v>0.72413793100000001</v>
+        <v>0.592592592592592</v>
       </c>
       <c r="I15" s="4">
-        <v>0.79310344799999999</v>
+        <v>0.592592592592592</v>
       </c>
       <c r="J15" s="4">
-        <v>0.76923076899999998</v>
+        <v>0.72413793103448199</v>
       </c>
       <c r="K15" s="4">
-        <v>0.46666666699999998</v>
+        <v>0.76923076923076905</v>
       </c>
       <c r="L15" s="4">
-        <v>0.2</v>
+        <v>0.73333333333333295</v>
       </c>
       <c r="M15" s="4">
-        <v>0.2</v>
+        <v>0.266666666666666</v>
       </c>
       <c r="N15" s="4">
-        <v>0.59689922500000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>0.266666666666666</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0.59842519685039297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B16" s="4">
-        <v>1.1938</v>
+        <v>0.99060000000000004</v>
       </c>
       <c r="C16" s="4">
-        <v>51.27</v>
+        <v>46.785713999999999</v>
       </c>
       <c r="D16" s="4">
         <v>5</v>
       </c>
-      <c r="E16" s="4">
-        <v>79.8</v>
-      </c>
-      <c r="F16" s="4">
-        <v>38.4</v>
-      </c>
-      <c r="G16" s="4">
-        <v>32</v>
+      <c r="E16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="H16" s="4">
-        <v>0.55172413799999998</v>
+        <v>0.44444444444444398</v>
       </c>
       <c r="I16" s="4">
-        <v>0.72413793100000001</v>
+        <v>0.44444444444444398</v>
       </c>
       <c r="J16" s="4">
-        <v>0.76923076899999998</v>
+        <v>0.51724137931034397</v>
       </c>
       <c r="K16" s="4">
-        <v>0.73333333300000003</v>
-      </c>
-      <c r="L16" s="4">
-        <v>0.26666666700000002</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0.26666666700000002</v>
-      </c>
-      <c r="N16" s="4">
-        <v>0.58914728699999996</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0.57317073170731703</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="C17" s="4">
+        <v>51.191667000000002</v>
+      </c>
+      <c r="D17" s="4">
+        <v>5</v>
+      </c>
+      <c r="E17" s="4">
+        <v>113.2</v>
+      </c>
+      <c r="F17" s="4">
+        <v>42.4</v>
+      </c>
+      <c r="G17" s="4">
+        <v>45.7</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0.37037037037037002</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0.37037037037037002</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0.68965517241379304</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0.52755905511810997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1.2192000000000001</v>
+      </c>
+      <c r="C18" s="4">
+        <v>46.307692000000003</v>
+      </c>
+      <c r="D18" s="4">
+        <v>4</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.62962962962962898</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0.62962962962962898</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.48275862068965503</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0.52439024390243905</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
         <v>25</v>
-      </c>
-      <c r="B17" s="4">
-        <v>4.9530000000000003</v>
-      </c>
-      <c r="C17" s="4">
-        <v>48.126984</v>
-      </c>
-      <c r="D17" s="4">
-        <v>4</v>
-      </c>
-      <c r="E17" s="4">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="F17" s="4">
-        <v>24.6</v>
-      </c>
-      <c r="G17" s="4">
-        <v>18.8</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0.96551724100000003</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0.58620689699999995</v>
-      </c>
-      <c r="J17" s="4">
-        <v>0.46153846199999998</v>
-      </c>
-      <c r="K17" s="4">
-        <v>1</v>
-      </c>
-      <c r="L17" s="4">
-        <v>0.133333333</v>
-      </c>
-      <c r="M17" s="4">
-        <v>6.6666666999999999E-2</v>
-      </c>
-      <c r="N17" s="4">
-        <v>0.58139534900000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="4">
-        <v>0.99060000000000004</v>
-      </c>
-      <c r="C18" s="4">
-        <v>46.785713999999999</v>
-      </c>
-      <c r="D18" s="4">
-        <v>5</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0.413793103</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0.517241379</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0.76923076899999998</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N18" s="4">
-        <v>0.55952380999999995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="4">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="C19" s="4">
-        <v>51.191667000000002</v>
       </c>
       <c r="D19" s="4">
         <v>5</v>
       </c>
-      <c r="E19" s="4">
-        <v>113.2</v>
-      </c>
-      <c r="F19" s="4">
-        <v>42.4</v>
-      </c>
-      <c r="G19" s="4">
-        <v>45.7</v>
-      </c>
-      <c r="H19" s="4">
-        <v>0.34482758600000002</v>
-      </c>
-      <c r="I19" s="4">
-        <v>0.68965517200000004</v>
+      <c r="E19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="J19" s="4">
-        <v>0.76923076899999998</v>
+        <v>0.24137931034482701</v>
       </c>
       <c r="K19" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="L19" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="M19" s="4">
-        <v>0.33333333300000001</v>
-      </c>
-      <c r="N19" s="4">
-        <v>0.51937984500000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="4">
+        <v>0.49090909090909002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="4">
-        <v>1.2192000000000001</v>
+        <v>25</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="C20" s="4">
-        <v>46.307692000000003</v>
+        <v>48.126984</v>
       </c>
       <c r="D20" s="4">
         <v>4</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" s="4">
-        <v>0.58620689699999995</v>
-      </c>
-      <c r="I20" s="4">
-        <v>0.482758621</v>
+      <c r="E20" s="4">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="F20" s="4">
+        <v>24.6</v>
+      </c>
+      <c r="G20" s="4">
+        <v>18.8</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="J20" s="4">
-        <v>0.46153846199999998</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>3</v>
+        <v>0.58620689655172398</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="L20" s="4">
+        <v>1</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0.133333333333333</v>
       </c>
       <c r="N20" s="4">
-        <v>0.51190476200000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="O20" s="4">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -1493,37 +1579,40 @@
         <v>3</v>
       </c>
       <c r="E21" s="4">
-        <v>101.1809524</v>
+        <v>101.18095238095199</v>
       </c>
       <c r="F21" s="4">
-        <v>58.142857139999997</v>
+        <v>58.142857142857103</v>
       </c>
       <c r="G21" s="4">
-        <v>79.866666670000001</v>
+        <v>79.866666666666603</v>
       </c>
       <c r="H21" s="4">
-        <v>0.20689655200000001</v>
+        <v>0.22222222222222199</v>
       </c>
       <c r="I21" s="4">
-        <v>0.27586206899999999</v>
+        <v>0.22222222222222199</v>
       </c>
       <c r="J21" s="4">
-        <v>0.34615384599999999</v>
+        <v>0.27586206896551702</v>
       </c>
       <c r="K21" s="4">
-        <v>0.53333333299999997</v>
+        <v>0.34615384615384598</v>
       </c>
       <c r="L21" s="4">
-        <v>0.73333333300000003</v>
+        <v>0.53333333333333299</v>
       </c>
       <c r="M21" s="4">
-        <v>0.73333333300000003</v>
+        <v>0.73333333333333295</v>
       </c>
       <c r="N21" s="4">
-        <v>0.41085271299999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="O21" s="4">
+        <v>0.41732283464566899</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1546,16 +1635,16 @@
         <v>3</v>
       </c>
       <c r="H22" s="4">
-        <v>0.37931034499999999</v>
+        <v>0.407407407407407</v>
       </c>
       <c r="I22" s="4">
-        <v>0.413793103</v>
+        <v>0.407407407407407</v>
       </c>
       <c r="J22" s="4">
-        <v>0.26923076899999998</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>3</v>
+        <v>0.41379310344827502</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0.269230769230769</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>3</v>
@@ -1563,11 +1652,14 @@
       <c r="M22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N22" s="4">
-        <v>0.35714285699999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="N22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O22" s="4">
+        <v>0.36585365853658502</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
@@ -1590,28 +1682,31 @@
         <v>25.6</v>
       </c>
       <c r="H23" s="4">
-        <v>0.44827586200000002</v>
+        <v>0.48148148148148101</v>
       </c>
       <c r="I23" s="4">
-        <v>0.34482758600000002</v>
+        <v>0.48148148148148101</v>
       </c>
       <c r="J23" s="4">
-        <v>0.26923076899999998</v>
+        <v>0.34482758620689602</v>
       </c>
       <c r="K23" s="4">
-        <v>0.73333333300000003</v>
+        <v>0.269230769230769</v>
       </c>
       <c r="L23" s="4">
-        <v>6.6666666999999999E-2</v>
+        <v>0.73333333333333295</v>
       </c>
       <c r="M23" s="4">
-        <v>0.133333333</v>
+        <v>6.6666666666666596E-2</v>
       </c>
       <c r="N23" s="4">
-        <v>0.34108527100000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="O23" s="4">
+        <v>0.34645669291338499</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
@@ -1625,37 +1720,40 @@
         <v>2</v>
       </c>
       <c r="E24" s="4">
-        <v>154.57142859999999</v>
+        <v>154.57142857142799</v>
       </c>
       <c r="F24" s="4">
-        <v>55.285714290000001</v>
+        <v>55.285714285714199</v>
       </c>
       <c r="G24" s="4">
         <v>71.7</v>
       </c>
       <c r="H24" s="4">
-        <v>0.27586206899999999</v>
+        <v>0.296296296296296</v>
       </c>
       <c r="I24" s="4">
-        <v>0.17241379300000001</v>
+        <v>0.296296296296296</v>
       </c>
       <c r="J24" s="4">
-        <v>0.26923076899999998</v>
+        <v>0.17241379310344801</v>
       </c>
       <c r="K24" s="4">
+        <v>0.269230769230769</v>
+      </c>
+      <c r="L24" s="4">
         <v>0.2</v>
       </c>
-      <c r="L24" s="4">
+      <c r="M24" s="4">
         <v>0.6</v>
       </c>
-      <c r="M24" s="4">
-        <v>0.53333333299999997</v>
-      </c>
       <c r="N24" s="4">
-        <v>0.31007751900000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="O24" s="4">
+        <v>0.31496062992125901</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="1" t="s">
         <v>15</v>
       </c>
@@ -1669,7 +1767,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="4">
-        <v>253.85714290000001</v>
+        <v>253.85714285714201</v>
       </c>
       <c r="F25" s="4">
         <v>40</v>
@@ -1678,28 +1776,31 @@
         <v>62.2</v>
       </c>
       <c r="H25" s="4">
-        <v>0.62068965499999995</v>
+        <v>0.66666666666666596</v>
       </c>
       <c r="I25" s="4">
-        <v>6.8965517000000004E-2</v>
+        <v>0.66666666666666596</v>
       </c>
       <c r="J25" s="4">
-        <v>7.6923077000000006E-2</v>
+        <v>6.8965517241379296E-2</v>
       </c>
       <c r="K25" s="4">
-        <v>6.6666666999999999E-2</v>
+        <v>7.69230769230769E-2</v>
       </c>
       <c r="L25" s="4">
-        <v>0.33333333300000001</v>
+        <v>6.6666666666666596E-2</v>
       </c>
       <c r="M25" s="4">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="N25" s="4">
         <v>0.4</v>
       </c>
-      <c r="N25" s="4">
-        <v>0.263565891</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="O25" s="4">
+        <v>0.26771653543307</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
@@ -1713,37 +1814,40 @@
         <v>1</v>
       </c>
       <c r="E26" s="4">
-        <v>182.85714290000001</v>
+        <v>182.85714285714201</v>
       </c>
       <c r="F26" s="4">
-        <v>48.428571429999998</v>
+        <v>48.428571428571402</v>
       </c>
       <c r="G26" s="4">
         <v>63.4</v>
       </c>
       <c r="H26" s="4">
-        <v>0.27586206899999999</v>
+        <v>0.296296296296296</v>
       </c>
       <c r="I26" s="4">
-        <v>0.20689655200000001</v>
+        <v>0.296296296296296</v>
       </c>
       <c r="J26" s="4">
-        <v>7.6923077000000006E-2</v>
+        <v>0.20689655172413701</v>
       </c>
       <c r="K26" s="4">
-        <v>0.133333333</v>
+        <v>7.69230769230769E-2</v>
       </c>
       <c r="L26" s="4">
-        <v>0.53333333299999997</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="M26" s="4">
-        <v>0.46666666699999998</v>
+        <v>0.53333333333333299</v>
       </c>
       <c r="N26" s="4">
-        <v>0.25581395299999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="O26" s="4">
+        <v>0.25984251968503902</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1766,16 +1870,16 @@
         <v>3</v>
       </c>
       <c r="H27" s="4">
-        <v>0.17241379300000001</v>
+        <v>0.18518518518518501</v>
       </c>
       <c r="I27" s="4">
-        <v>0.31034482800000002</v>
+        <v>0.18518518518518501</v>
       </c>
       <c r="J27" s="4">
-        <v>0.26923076899999998</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>3</v>
+        <v>0.31034482758620602</v>
+      </c>
+      <c r="K27" s="4">
+        <v>0.269230769230769</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>3</v>
@@ -1783,11 +1887,14 @@
       <c r="M27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N27" s="4">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="N27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O27" s="4">
+        <v>0.25609756097560898</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
@@ -1810,13 +1917,13 @@
         <v>3</v>
       </c>
       <c r="H28" s="4">
-        <v>3.4482759000000002E-2</v>
+        <v>3.7037037037037E-2</v>
       </c>
       <c r="I28" s="4">
-        <v>0.37931034499999999</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>3</v>
+        <v>3.7037037037037E-2</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0.37931034482758602</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>3</v>
@@ -1827,11 +1934,14 @@
       <c r="M28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N28" s="4">
-        <v>0.20689655200000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="N28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O28" s="4">
+        <v>0.214285714285714</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -1854,16 +1964,16 @@
         <v>3</v>
       </c>
       <c r="H29" s="4">
-        <v>0.13793103400000001</v>
+        <v>0.148148148148148</v>
       </c>
       <c r="I29" s="4">
-        <v>0.10344827600000001</v>
+        <v>0.148148148148148</v>
       </c>
       <c r="J29" s="4">
-        <v>0.26923076899999998</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>3</v>
+        <v>0.10344827586206801</v>
+      </c>
+      <c r="K29" s="4">
+        <v>0.269230769230769</v>
       </c>
       <c r="L29" s="4" t="s">
         <v>3</v>
@@ -1871,11 +1981,14 @@
       <c r="M29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N29" s="4">
-        <v>0.16666666699999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="N29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O29" s="4">
+        <v>0.17073170731707299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -1898,13 +2011,13 @@
         <v>3</v>
       </c>
       <c r="H30" s="4">
-        <v>0.13793103400000001</v>
+        <v>0.148148148148148</v>
       </c>
       <c r="I30" s="4">
-        <v>0.13793103400000001</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>3</v>
+        <v>0.148148148148148</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0.13793103448275801</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>3</v>
@@ -1915,11 +2028,14 @@
       <c r="M30" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N30" s="4">
-        <v>0.13793103400000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="N30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O30" s="4">
+        <v>0.14285714285714199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -1942,13 +2058,13 @@
         <v>3</v>
       </c>
       <c r="H31" s="4">
-        <v>0.13793103400000001</v>
+        <v>0.148148148148148</v>
       </c>
       <c r="I31" s="4">
-        <v>3.4482759000000002E-2</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>3</v>
+        <v>0.148148148148148</v>
+      </c>
+      <c r="J31" s="4">
+        <v>3.4482758620689599E-2</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>3</v>
@@ -1959,16 +2075,19 @@
       <c r="M31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N31" s="4">
-        <v>8.6206897000000005E-2</v>
+      <c r="N31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O31" s="4">
+        <v>8.9285714285714302E-2</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:N27">
-    <sortCondition descending="1" ref="N3"/>
+  <sortState ref="A3:O27">
+    <sortCondition descending="1" ref="O3"/>
   </sortState>
   <mergeCells count="2">
-    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="I1:N1"/>
     <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
AFE update. New FRS calculation based on percent of range rather than quantiles.
</commit_message>
<xml_diff>
--- a/manuscript/tables/TableS1.xlsx
+++ b/manuscript/tables/TableS1.xlsx
@@ -1,15 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jens/Documents/Davis/Post-Doc/FireTraits/fire_traits/manuscript/tables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9087BBAA-30AE-EF4A-B342-601151D44F99}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableS1.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="TableS1_v2.csv (2)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="40">
   <si>
     <t>Scientific_Name</t>
   </si>
@@ -144,11 +151,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -247,19 +254,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -304,6 +311,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -628,14 +643,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:O31"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
@@ -655,23 +670,23 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="5" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="7"/>
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="33" customHeight="1">
@@ -2098,4 +2113,1382 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43675B33-0688-A745-81E3-013A0EAF03EE}">
+  <dimension ref="A1:O31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="8" max="8" width="1.6640625" customWidth="1"/>
+    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="1"/>
+      <c r="B1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" ht="33" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2.0573999999999999</v>
+      </c>
+      <c r="C3" s="4">
+        <v>95.165216999999998</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="F3" s="4">
+        <v>59.4</v>
+      </c>
+      <c r="G3" s="4">
+        <v>86.1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0.73731343283581996</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0.93521877546415499</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0.92464878671775197</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0.83291692451238897</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1.7272000000000001</v>
+      </c>
+      <c r="C4" s="4">
+        <v>51.416666999999997</v>
+      </c>
+      <c r="D4" s="4">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4">
+        <v>79.2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>67.3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>90</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.77966101694915202</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.47657856097141799</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.85522388059701404</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.90516028727952302</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0.974457215836526</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0.80880303628967098</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2.0573999999999999</v>
+      </c>
+      <c r="C5" s="4">
+        <v>85.578946999999999</v>
+      </c>
+      <c r="D5" s="4">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4">
+        <v>148.5</v>
+      </c>
+      <c r="F5" s="4">
+        <v>42.6</v>
+      </c>
+      <c r="G5" s="4">
+        <v>75.8</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.88530684472247601</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0.77777777777777701</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.48656716417910401</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0.54601317845279895</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.79310344827586199</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0.78844736820023398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1.6002000000000001</v>
+      </c>
+      <c r="C6" s="4">
+        <v>41.229047999999999</v>
+      </c>
+      <c r="D6" s="4">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4">
+        <v>79.7</v>
+      </c>
+      <c r="F6" s="4">
+        <v>77</v>
+      </c>
+      <c r="G6" s="4">
+        <v>92</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.69491525423728795</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.35469067674999999</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0.90256903829808899</v>
+      </c>
+      <c r="N6" s="4">
+        <v>1</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0.78429390082519101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1.8288</v>
+      </c>
+      <c r="C7" s="4">
+        <v>62.285713999999999</v>
+      </c>
+      <c r="D7" s="4">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4">
+        <v>128.5</v>
+      </c>
+      <c r="F7" s="4">
+        <v>55.6</v>
+      </c>
+      <c r="G7" s="4">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.84745762711864403</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.60661926452866199</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.68059701492537295</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0.64966313771015105</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.80970625798211904</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0.780797721686327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1.6002000000000001</v>
+      </c>
+      <c r="C8" s="4">
+        <v>51.095238000000002</v>
+      </c>
+      <c r="D8" s="4">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.69491525423728795</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.47273288312093997</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.88888888888888795</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0.68551234208237199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2.0573999999999999</v>
+      </c>
+      <c r="C9" s="4">
+        <v>50</v>
+      </c>
+      <c r="D9" s="4">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.45962911053787597</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.55555555555555503</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0.67172822203114402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="C10" s="4">
+        <v>62.133333</v>
+      </c>
+      <c r="D10" s="4">
+        <v>6</v>
+      </c>
+      <c r="E10" s="4">
+        <v>90.29</v>
+      </c>
+      <c r="F10" s="4">
+        <v>75.14</v>
+      </c>
+      <c r="G10" s="4">
+        <v>82.78</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.22033898305084701</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.60479613022362499</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0.55555555555555503</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0.972238805970149</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0.84768638487132097</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0.88224776500638502</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0.61685034584915899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1.524</v>
+      </c>
+      <c r="C11" s="4">
+        <v>48.083333000000003</v>
+      </c>
+      <c r="D11" s="4">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.644067796610169</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.436697502535358</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0.50840324786332403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1.6002000000000001</v>
+      </c>
+      <c r="C12" s="4">
+        <v>54.256194000000001</v>
+      </c>
+      <c r="D12" s="4">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4">
+        <v>105.8</v>
+      </c>
+      <c r="F12" s="4">
+        <v>26.2</v>
+      </c>
+      <c r="G12" s="4">
+        <v>26.6</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0.69491525423728795</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.51055155684215003</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0.24179104477611901</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0.76730584146724501</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0.16475095785440599</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0.49354808826486601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1.1938</v>
+      </c>
+      <c r="C13" s="4">
+        <v>51.27</v>
+      </c>
+      <c r="D13" s="4">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4">
+        <v>79.8</v>
+      </c>
+      <c r="F13" s="4">
+        <v>38.4</v>
+      </c>
+      <c r="G13" s="4">
+        <v>32</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0.42372881355932202</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.47482379076307901</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0.42388059701492498</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0.90205078850180198</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0.233716475095785</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0.47334281617806401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1.143</v>
+      </c>
+      <c r="C14" s="4">
+        <v>55.122799999999998</v>
+      </c>
+      <c r="D14" s="4">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.38983050847457601</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0.52091990412659195</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0.45173161901520398</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1.1684000000000001</v>
+      </c>
+      <c r="C15" s="4">
+        <v>59.424999999999997</v>
+      </c>
+      <c r="D15" s="4">
+        <v>4</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0.40677966101694901</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.57239278071310196</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0.437501925021128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="C16" s="4">
+        <v>51.191667000000002</v>
+      </c>
+      <c r="D16" s="4">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4">
+        <v>113.2</v>
+      </c>
+      <c r="F16" s="4">
+        <v>42.4</v>
+      </c>
+      <c r="G16" s="4">
+        <v>45.7</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0.22033898305084701</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.47388659006537798</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0.48358208955223803</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0.72895535654202503</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0.40868454661558101</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0.43674801772308802</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1.2192000000000001</v>
+      </c>
+      <c r="C17" s="4">
+        <v>46.307692000000003</v>
+      </c>
+      <c r="D17" s="4">
+        <v>4</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0.44067796610169502</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0.41545317403948401</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0.39648815782483698</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.71120000000000005</v>
+      </c>
+      <c r="C18" s="4">
+        <v>26.055555999999999</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3</v>
+      </c>
+      <c r="E18" s="4">
+        <v>101.18095238666599</v>
+      </c>
+      <c r="F18" s="4">
+        <v>58.142857143333302</v>
+      </c>
+      <c r="G18" s="4">
+        <v>79.866666666666603</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0.101694915254237</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.17315023671876001</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0.71855010661691499</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0.79124404631373302</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0.84504044274159196</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0.38586894357346102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.99060000000000004</v>
+      </c>
+      <c r="C19" s="4">
+        <v>46.785713999999999</v>
+      </c>
+      <c r="D19" s="4">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0.28813559322033899</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.42117237989035999</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="4">
+        <v>0.38458413918504702</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="C20" s="4">
+        <v>48.126984</v>
+      </c>
+      <c r="D20" s="4">
+        <v>4</v>
+      </c>
+      <c r="E20" s="4">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="F20" s="4">
+        <v>24.6</v>
+      </c>
+      <c r="G20" s="4">
+        <v>18.8</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0.305084745762711</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.43721975685544401</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0.217910447761194</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0.96113126527849302</v>
+      </c>
+      <c r="N20" s="4">
+        <v>6.5134099616858204E-2</v>
+      </c>
+      <c r="O20" s="4">
+        <v>0.37852081663035497</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="C21" s="4">
+        <v>25</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0.305084745762711</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.16052123208900099</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O21" s="4">
+        <v>0.30335014076538502</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="C22" s="4">
+        <v>17.142856999999999</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4">
+        <v>154.57142859999999</v>
+      </c>
+      <c r="F22" s="4">
+        <v>55.285714290000001</v>
+      </c>
+      <c r="G22" s="4">
+        <v>71.7</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0.13559322033898299</v>
+      </c>
+      <c r="J22" s="4">
+        <v>6.6515897153024195E-2</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0.67590618343283504</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0.51454801210160295</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0.74074074074074003</v>
+      </c>
+      <c r="O22" s="4">
+        <v>0.29616670822143198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.55879999999999996</v>
+      </c>
+      <c r="C23" s="4">
+        <v>35.4375</v>
+      </c>
+      <c r="D23" s="4">
+        <v>6</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.28539877134140601</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0.55555555555555503</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O23" s="4">
+        <v>0.28031810896565401</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1.0414000000000001</v>
+      </c>
+      <c r="C24" s="4">
+        <v>27.410506000000002</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>79.8</v>
+      </c>
+      <c r="F24" s="4">
+        <v>16.7</v>
+      </c>
+      <c r="G24" s="4">
+        <v>25.6</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0.322033898305084</v>
+      </c>
+      <c r="J24" s="4">
+        <v>0.189361285514932</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="L24" s="4">
+        <v>9.9999999999999895E-2</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0.90205078850180198</v>
+      </c>
+      <c r="N24" s="4">
+        <v>0.151979565772669</v>
+      </c>
+      <c r="O24" s="4">
+        <v>0.27049754238069801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="C25" s="4">
+        <v>17.585764999999999</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4">
+        <v>182.85714290000001</v>
+      </c>
+      <c r="F25" s="4">
+        <v>48.428571429999998</v>
+      </c>
+      <c r="G25" s="4">
+        <v>63.4</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0.13559322033898299</v>
+      </c>
+      <c r="J25" s="4">
+        <v>7.1814988042145506E-2</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0</v>
+      </c>
+      <c r="L25" s="4">
+        <v>0.57356076761193997</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0.36795735536359803</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0.63473818646232405</v>
+      </c>
+      <c r="O25" s="4">
+        <v>0.231369918474507</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.91439999999999999</v>
+      </c>
+      <c r="C26" s="4">
+        <v>37.192999999999998</v>
+      </c>
+      <c r="D26" s="4">
+        <v>2</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0.23728813559322001</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.30640212656608601</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O26" s="4">
+        <v>0.21826712442347199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.68579999999999997</v>
+      </c>
+      <c r="C27" s="4">
+        <v>27.081022000000001</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2</v>
+      </c>
+      <c r="E27" s="4">
+        <v>60.9</v>
+      </c>
+      <c r="F27" s="4">
+        <v>10</v>
+      </c>
+      <c r="G27" s="4">
+        <v>13.7</v>
+      </c>
+      <c r="I27" s="4">
+        <v>8.4745762711864403E-2</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0.18541923510601799</v>
+      </c>
+      <c r="K27" s="4">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="L27" s="4">
+        <v>0</v>
+      </c>
+      <c r="M27" s="4">
+        <v>1</v>
+      </c>
+      <c r="N27" s="4">
+        <v>0</v>
+      </c>
+      <c r="O27" s="4">
+        <v>0.20042227525141301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.81279999999999997</v>
+      </c>
+      <c r="C28" s="4">
+        <v>13.53</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1</v>
+      </c>
+      <c r="E28" s="4">
+        <v>253.85714290000001</v>
+      </c>
+      <c r="F28" s="4">
+        <v>40</v>
+      </c>
+      <c r="G28" s="4">
+        <v>62.2</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0.169491525423728</v>
+      </c>
+      <c r="J28" s="4">
+        <v>2.3290537456657399E-2</v>
+      </c>
+      <c r="K28" s="4">
+        <v>0</v>
+      </c>
+      <c r="L28" s="4">
+        <v>0.44776119402984998</v>
+      </c>
+      <c r="M28" s="4">
+        <v>0</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0.61941251596423996</v>
+      </c>
+      <c r="O28" s="4">
+        <v>0.16789229024767799</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.83819999999999995</v>
+      </c>
+      <c r="C29" s="4">
+        <v>11.583333</v>
+      </c>
+      <c r="D29" s="4">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0.186440677966101</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O29" s="4">
+        <v>9.9183929692404194E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="C30" s="4">
+        <v>16.256153999999999</v>
+      </c>
+      <c r="D30" s="4">
+        <v>2</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="4">
+        <v>5.0847457627118599E-2</v>
+      </c>
+      <c r="J30" s="4">
+        <v>5.5907103027253997E-2</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O30" s="4">
+        <v>7.2621890588494595E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="C31" s="4">
+        <v>15.871333999999999</v>
+      </c>
+      <c r="D31" s="4">
+        <v>2</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="4">
+        <v>5.0847457627118599E-2</v>
+      </c>
+      <c r="J31" s="4">
+        <v>5.1302995275866202E-2</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O31" s="4">
+        <v>7.1087188004698598E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="I1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Major update, incorporating new full flammability dataset into analysis (table 1 and cluster figure)
</commit_message>
<xml_diff>
--- a/manuscript/tables/TableS1.xlsx
+++ b/manuscript/tables/TableS1.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jens/Documents/Davis/Post-Doc/FireTraits/fire_traits/manuscript/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9087BBAA-30AE-EF4A-B342-601151D44F99}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D6D3967F-04F0-D248-81CD-C04E418656C1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TableS1.csv" sheetId="1" r:id="rId1"/>
-    <sheet name="TableS1_v2.csv (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="TableS1.csv_quantile" sheetId="1" r:id="rId1"/>
+    <sheet name="TableS1_v2.csv_percent of range" sheetId="2" r:id="rId2"/>
+    <sheet name="TableS1_percent of range_full" sheetId="4" r:id="rId3"/>
+    <sheet name="TableS1_PctOfRange_full_PC" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="87">
   <si>
     <t>Scientific_Name</t>
   </si>
@@ -146,6 +148,147 @@
   </si>
   <si>
     <t>Juniperus_scopulorum</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Plant.height</t>
+  </si>
+  <si>
+    <t>Self.pruning</t>
+  </si>
+  <si>
+    <t>Flame_duration</t>
+  </si>
+  <si>
+    <t>Flame_ht</t>
+  </si>
+  <si>
+    <t>Pct_consumed</t>
+  </si>
+  <si>
+    <t>log_Bark.thickness</t>
+  </si>
+  <si>
+    <t>log_Flame_duration</t>
+  </si>
+  <si>
+    <t>Pin_Pon</t>
+  </si>
+  <si>
+    <t>Pin_Mon3</t>
+  </si>
+  <si>
+    <t>Pin_Jef</t>
+  </si>
+  <si>
+    <t>Seq_Sem</t>
+  </si>
+  <si>
+    <t>Pin_Con</t>
+  </si>
+  <si>
+    <t>Pin_Lam</t>
+  </si>
+  <si>
+    <t>Pin_Fle</t>
+  </si>
+  <si>
+    <t>Pin_Alb</t>
+  </si>
+  <si>
+    <t>Cha_Noo</t>
+  </si>
+  <si>
+    <t>Seq_Gig</t>
+  </si>
+  <si>
+    <t>Thu_Pli</t>
+  </si>
+  <si>
+    <t>Pin_Edu</t>
+  </si>
+  <si>
+    <t>Abi_Ama</t>
+  </si>
+  <si>
+    <t>Jun_Sco</t>
+  </si>
+  <si>
+    <t>Lar_Occ</t>
+  </si>
+  <si>
+    <t>Pse_Men</t>
+  </si>
+  <si>
+    <t>Jun_Occ</t>
+  </si>
+  <si>
+    <t>Cal_Dec</t>
+  </si>
+  <si>
+    <t>Tsu_Het</t>
+  </si>
+  <si>
+    <t>Abi_Con</t>
+  </si>
+  <si>
+    <t>Cha_Law</t>
+  </si>
+  <si>
+    <t>Abi_Mag</t>
+  </si>
+  <si>
+    <t>Abi_Las</t>
+  </si>
+  <si>
+    <t>Pic_Gla</t>
+  </si>
+  <si>
+    <t>Tsu_Mer</t>
+  </si>
+  <si>
+    <t>Abi_Gra</t>
+  </si>
+  <si>
+    <t>Abi_Pro</t>
+  </si>
+  <si>
+    <t>Pic_Sit</t>
+  </si>
+  <si>
+    <t>Pic_Eng</t>
+  </si>
+  <si>
+    <t>Percentile of range</t>
+  </si>
+  <si>
+    <t>bt.pct</t>
+  </si>
+  <si>
+    <t>ph.pct</t>
+  </si>
+  <si>
+    <t>sp.pct</t>
+  </si>
+  <si>
+    <t>fh_pc.pct</t>
+  </si>
+  <si>
+    <t>fd.pct</t>
+  </si>
+  <si>
+    <t>fh.pct</t>
+  </si>
+  <si>
+    <t>pc.pct</t>
+  </si>
+  <si>
+    <t>frs</t>
+  </si>
+  <si>
+    <t>BT</t>
   </si>
 </sst>
 </file>
@@ -155,7 +298,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,6 +326,24 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times Roman"/>
     </font>
   </fonts>
   <fills count="2">
@@ -250,7 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -269,6 +430,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -646,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:N31"/>
+    <sheetView showRuler="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2119,8 +2284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43675B33-0688-A745-81E3-013A0EAF03EE}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2153,7 +2318,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="5"/>
       <c r="I1" s="6" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -3491,4 +3656,3414 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D59AA44-26EB-D747-B5F7-C7997FFD20FF}">
+  <dimension ref="A1:R31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:R1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="11">
+        <v>2.0573999999999999</v>
+      </c>
+      <c r="D3" s="11">
+        <v>95.165220000000005</v>
+      </c>
+      <c r="E3" s="11">
+        <v>5</v>
+      </c>
+      <c r="F3" s="11">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="G3" s="11">
+        <v>59.4</v>
+      </c>
+      <c r="H3" s="11">
+        <v>86.1</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0.31331873500000001</v>
+      </c>
+      <c r="J3" s="11">
+        <v>1.865696</v>
+      </c>
+      <c r="K3" s="11">
+        <v>1</v>
+      </c>
+      <c r="L3" s="11">
+        <v>1</v>
+      </c>
+      <c r="M3" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N3" s="11">
+        <v>0.84988505999999997</v>
+      </c>
+      <c r="O3" s="11">
+        <v>0.86922189999999999</v>
+      </c>
+      <c r="P3" s="11">
+        <v>0.73731343000000005</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>0.92464878699999997</v>
+      </c>
+      <c r="R3" s="11">
+        <v>0.82927139999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="11">
+        <v>1.7272000000000001</v>
+      </c>
+      <c r="D4" s="11">
+        <v>51.416670000000003</v>
+      </c>
+      <c r="E4" s="11">
+        <v>10</v>
+      </c>
+      <c r="F4" s="11">
+        <v>79.2</v>
+      </c>
+      <c r="G4" s="11">
+        <v>67.3</v>
+      </c>
+      <c r="H4" s="11">
+        <v>90</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.237342629</v>
+      </c>
+      <c r="J4" s="11">
+        <v>1.898725</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0.77966102000000004</v>
+      </c>
+      <c r="L4" s="11">
+        <v>0.47657855999999998</v>
+      </c>
+      <c r="M4" s="11">
+        <v>1</v>
+      </c>
+      <c r="N4" s="11">
+        <v>0.92687235000000001</v>
+      </c>
+      <c r="O4" s="11">
+        <v>0.81594670000000002</v>
+      </c>
+      <c r="P4" s="11">
+        <v>0.85522388000000005</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>0.97445721600000001</v>
+      </c>
+      <c r="R4" s="11">
+        <v>0.81697790000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1.6002000000000001</v>
+      </c>
+      <c r="D5" s="11">
+        <v>41.229050000000001</v>
+      </c>
+      <c r="E5" s="11">
+        <v>10</v>
+      </c>
+      <c r="F5" s="11">
+        <v>79.7</v>
+      </c>
+      <c r="G5" s="11">
+        <v>77</v>
+      </c>
+      <c r="H5" s="11">
+        <v>92</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0.20417426599999999</v>
+      </c>
+      <c r="J5" s="11">
+        <v>1.9014580000000001</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0.69491524999999998</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0.35469067999999998</v>
+      </c>
+      <c r="M5" s="11">
+        <v>1</v>
+      </c>
+      <c r="N5" s="11">
+        <v>1</v>
+      </c>
+      <c r="O5" s="11">
+        <v>0.81153819999999999</v>
+      </c>
+      <c r="P5" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>1</v>
+      </c>
+      <c r="R5" s="11">
+        <v>0.81019070000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1.8288</v>
+      </c>
+      <c r="D6" s="11">
+        <v>62.285710000000002</v>
+      </c>
+      <c r="E6" s="11">
+        <v>10</v>
+      </c>
+      <c r="F6" s="11">
+        <v>128.5</v>
+      </c>
+      <c r="G6" s="11">
+        <v>55.6</v>
+      </c>
+      <c r="H6" s="11">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0.26216621299999998</v>
+      </c>
+      <c r="J6" s="11">
+        <v>2.1089030000000002</v>
+      </c>
+      <c r="K6" s="11">
+        <v>0.84745762999999996</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0.60661925999999999</v>
+      </c>
+      <c r="M6" s="11">
+        <v>1</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0.75818001000000002</v>
+      </c>
+      <c r="O6" s="11">
+        <v>0.47693479999999999</v>
+      </c>
+      <c r="P6" s="11">
+        <v>0.68059700999999995</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>0.80970625799999996</v>
+      </c>
+      <c r="R6" s="11">
+        <v>0.73688580000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2.0573999999999999</v>
+      </c>
+      <c r="D7" s="11">
+        <v>85.578950000000006</v>
+      </c>
+      <c r="E7" s="11">
+        <v>8</v>
+      </c>
+      <c r="F7" s="11">
+        <v>148.5</v>
+      </c>
+      <c r="G7" s="11">
+        <v>42.6</v>
+      </c>
+      <c r="H7" s="11">
+        <v>75.8</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.31331873500000001</v>
+      </c>
+      <c r="J7" s="11">
+        <v>2.171726</v>
+      </c>
+      <c r="K7" s="11">
+        <v>1</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0.88530684000000004</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0.77777779999999996</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0.67076778999999997</v>
+      </c>
+      <c r="O7" s="11">
+        <v>0.3756023</v>
+      </c>
+      <c r="P7" s="11">
+        <v>0.48656716</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>0.79310344799999999</v>
+      </c>
+      <c r="R7" s="11">
+        <v>0.71972630000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="D8" s="11">
+        <v>62.133330000000001</v>
+      </c>
+      <c r="E8" s="11">
+        <v>6</v>
+      </c>
+      <c r="F8" s="11">
+        <v>90.29</v>
+      </c>
+      <c r="G8" s="11">
+        <v>75.14</v>
+      </c>
+      <c r="H8" s="11">
+        <v>82.78</v>
+      </c>
+      <c r="I8" s="11">
+        <v>-5.1098238999999997E-2</v>
+      </c>
+      <c r="J8" s="11">
+        <v>1.95564</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0.22033897999999999</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0.60479612999999999</v>
+      </c>
+      <c r="M8" s="11">
+        <v>0.55555560000000004</v>
+      </c>
+      <c r="N8" s="11">
+        <v>0.91816231999999998</v>
+      </c>
+      <c r="O8" s="11">
+        <v>0.72414509999999999</v>
+      </c>
+      <c r="P8" s="11">
+        <v>0.97223881000000001</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>0.88224776500000002</v>
+      </c>
+      <c r="R8" s="11">
+        <v>0.65988709999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1.6002000000000001</v>
+      </c>
+      <c r="D9" s="11">
+        <v>51.095239999999997</v>
+      </c>
+      <c r="E9" s="11">
+        <v>9</v>
+      </c>
+      <c r="F9" s="11">
+        <v>89.857140000000001</v>
+      </c>
+      <c r="G9" s="11">
+        <v>27.86</v>
+      </c>
+      <c r="H9" s="11">
+        <v>34.590000000000003</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0.20417426599999999</v>
+      </c>
+      <c r="J9" s="11">
+        <v>1.9535530000000001</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0.69491524999999998</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0.47273288000000002</v>
+      </c>
+      <c r="M9" s="11">
+        <v>0.88888889999999998</v>
+      </c>
+      <c r="N9" s="11">
+        <v>0.26670369999999999</v>
+      </c>
+      <c r="O9" s="11">
+        <v>0.72751140000000003</v>
+      </c>
+      <c r="P9" s="11">
+        <v>0.26656716000000003</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>0.26679438100000002</v>
+      </c>
+      <c r="R9" s="11">
+        <v>0.55290170000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="11">
+        <v>2.0573999999999999</v>
+      </c>
+      <c r="D10" s="11">
+        <v>50</v>
+      </c>
+      <c r="E10" s="11">
+        <v>6</v>
+      </c>
+      <c r="F10" s="11">
+        <v>115.57143000000001</v>
+      </c>
+      <c r="G10" s="11">
+        <v>21.71</v>
+      </c>
+      <c r="H10" s="11">
+        <v>31.37</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0.31331873500000001</v>
+      </c>
+      <c r="J10" s="11">
+        <v>2.0628500000000001</v>
+      </c>
+      <c r="K10" s="11">
+        <v>1</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0.45962911000000001</v>
+      </c>
+      <c r="M10" s="11">
+        <v>0.55555560000000004</v>
+      </c>
+      <c r="N10" s="11">
+        <v>0.20535903999999999</v>
+      </c>
+      <c r="O10" s="11">
+        <v>0.55121659999999995</v>
+      </c>
+      <c r="P10" s="11">
+        <v>0.17477612000000001</v>
+      </c>
+      <c r="Q10" s="11">
+        <v>0.225670498</v>
+      </c>
+      <c r="R10" s="11">
+        <v>0.49447459999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="11">
+        <v>1.1938</v>
+      </c>
+      <c r="D11" s="11">
+        <v>51.27</v>
+      </c>
+      <c r="E11" s="11">
+        <v>5</v>
+      </c>
+      <c r="F11" s="11">
+        <v>79.8</v>
+      </c>
+      <c r="G11" s="11">
+        <v>38.4</v>
+      </c>
+      <c r="H11" s="11">
+        <v>32</v>
+      </c>
+      <c r="I11" s="11">
+        <v>7.6931575000000002E-2</v>
+      </c>
+      <c r="J11" s="11">
+        <v>1.9020030000000001</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0.42372881000000001</v>
+      </c>
+      <c r="L11" s="11">
+        <v>0.47482379000000002</v>
+      </c>
+      <c r="M11" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N11" s="11">
+        <v>0.30960913000000001</v>
+      </c>
+      <c r="O11" s="11">
+        <v>0.81065989999999999</v>
+      </c>
+      <c r="P11" s="11">
+        <v>0.4238806</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>0.23371647500000001</v>
+      </c>
+      <c r="R11" s="11">
+        <v>0.46854230000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1.524</v>
+      </c>
+      <c r="D12" s="11">
+        <v>48.083329999999997</v>
+      </c>
+      <c r="E12" s="11">
+        <v>5</v>
+      </c>
+      <c r="F12" s="11">
+        <v>105</v>
+      </c>
+      <c r="G12" s="11">
+        <v>25.29</v>
+      </c>
+      <c r="H12" s="11">
+        <v>46.64</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0.182984967</v>
+      </c>
+      <c r="J12" s="11">
+        <v>2.0211890000000001</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0.64406779999999997</v>
+      </c>
+      <c r="L12" s="11">
+        <v>0.43669750000000002</v>
+      </c>
+      <c r="M12" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N12" s="11">
+        <v>0.34387246999999999</v>
+      </c>
+      <c r="O12" s="11">
+        <v>0.6184151</v>
+      </c>
+      <c r="P12" s="11">
+        <v>0.22820895999999999</v>
+      </c>
+      <c r="Q12" s="11">
+        <v>0.420689655</v>
+      </c>
+      <c r="R12" s="11">
+        <v>0.46542060000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0.71120000000000005</v>
+      </c>
+      <c r="D13" s="11">
+        <v>26.05556</v>
+      </c>
+      <c r="E13" s="11">
+        <v>3</v>
+      </c>
+      <c r="F13" s="11">
+        <v>101.18095</v>
+      </c>
+      <c r="G13" s="11">
+        <v>58.142859999999999</v>
+      </c>
+      <c r="H13" s="11">
+        <v>79.866669999999999</v>
+      </c>
+      <c r="I13" s="11">
+        <v>-0.14800825200000001</v>
+      </c>
+      <c r="J13" s="11">
+        <v>2.005099</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0.10169491999999999</v>
+      </c>
+      <c r="L13" s="11">
+        <v>0.17315024000000001</v>
+      </c>
+      <c r="M13" s="11">
+        <v>0.22222220000000001</v>
+      </c>
+      <c r="N13" s="11">
+        <v>0.79455938000000004</v>
+      </c>
+      <c r="O13" s="11">
+        <v>0.64436870000000002</v>
+      </c>
+      <c r="P13" s="11">
+        <v>0.71855011000000002</v>
+      </c>
+      <c r="Q13" s="11">
+        <v>0.84504044300000003</v>
+      </c>
+      <c r="R13" s="11">
+        <v>0.45083780000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="11">
+        <v>1.6002000000000001</v>
+      </c>
+      <c r="D14" s="11">
+        <v>54.256189999999997</v>
+      </c>
+      <c r="E14" s="11">
+        <v>5</v>
+      </c>
+      <c r="F14" s="11">
+        <v>105.8</v>
+      </c>
+      <c r="G14" s="11">
+        <v>26.2</v>
+      </c>
+      <c r="H14" s="11">
+        <v>26.6</v>
+      </c>
+      <c r="I14" s="11">
+        <v>0.20417426599999999</v>
+      </c>
+      <c r="J14" s="11">
+        <v>2.024486</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0.69491524999999998</v>
+      </c>
+      <c r="L14" s="11">
+        <v>0.51055156000000002</v>
+      </c>
+      <c r="M14" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0.19549691</v>
+      </c>
+      <c r="O14" s="11">
+        <v>0.61309809999999998</v>
+      </c>
+      <c r="P14" s="11">
+        <v>0.24179104000000001</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>0.164750958</v>
+      </c>
+      <c r="R14" s="11">
+        <v>0.44492520000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="D15" s="11">
+        <v>51.191670000000002</v>
+      </c>
+      <c r="E15" s="11">
+        <v>5</v>
+      </c>
+      <c r="F15" s="11">
+        <v>113.2</v>
+      </c>
+      <c r="G15" s="11">
+        <v>42.4</v>
+      </c>
+      <c r="H15" s="11">
+        <v>45.7</v>
+      </c>
+      <c r="I15" s="11">
+        <v>-5.1098238999999997E-2</v>
+      </c>
+      <c r="J15" s="11">
+        <v>2.0538460000000001</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0.22033897999999999</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0.47388659</v>
+      </c>
+      <c r="M15" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N15" s="11">
+        <v>0.43857542999999999</v>
+      </c>
+      <c r="O15" s="11">
+        <v>0.56573989999999996</v>
+      </c>
+      <c r="P15" s="11">
+        <v>0.48358209000000002</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>0.40868454700000001</v>
+      </c>
+      <c r="R15" s="11">
+        <v>0.43277939999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0.55879999999999996</v>
+      </c>
+      <c r="D16" s="11">
+        <v>35.4375</v>
+      </c>
+      <c r="E16" s="11">
+        <v>6</v>
+      </c>
+      <c r="F16" s="11">
+        <v>134.14286000000001</v>
+      </c>
+      <c r="G16" s="11">
+        <v>48</v>
+      </c>
+      <c r="H16" s="11">
+        <v>65.69</v>
+      </c>
+      <c r="I16" s="11">
+        <v>-0.25274360299999998</v>
+      </c>
+      <c r="J16" s="11">
+        <v>2.1275680000000001</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0.28539877000000002</v>
+      </c>
+      <c r="M16" s="11">
+        <v>0.55555560000000004</v>
+      </c>
+      <c r="N16" s="11">
+        <v>0.62534455</v>
+      </c>
+      <c r="O16" s="11">
+        <v>0.44682949999999999</v>
+      </c>
+      <c r="P16" s="11">
+        <v>0.56716418000000002</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>0.66398467400000005</v>
+      </c>
+      <c r="R16" s="11">
+        <v>0.41982209999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="11">
+        <v>1.2192000000000001</v>
+      </c>
+      <c r="D17" s="11">
+        <v>46.307690000000001</v>
+      </c>
+      <c r="E17" s="11">
+        <v>4</v>
+      </c>
+      <c r="F17" s="11">
+        <v>97.285709999999995</v>
+      </c>
+      <c r="G17" s="11">
+        <v>22.86</v>
+      </c>
+      <c r="H17" s="11">
+        <v>44.54</v>
+      </c>
+      <c r="I17" s="11">
+        <v>8.6074953999999995E-2</v>
+      </c>
+      <c r="J17" s="11">
+        <v>1.988049</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0.44067796999999997</v>
+      </c>
+      <c r="L17" s="11">
+        <v>0.41545316999999998</v>
+      </c>
+      <c r="M17" s="11">
+        <v>0.3333333</v>
+      </c>
+      <c r="N17" s="11">
+        <v>0.31328165000000002</v>
+      </c>
+      <c r="O17" s="11">
+        <v>0.67186950000000001</v>
+      </c>
+      <c r="P17" s="11">
+        <v>0.19194030000000001</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>0.39386973199999997</v>
+      </c>
+      <c r="R17" s="11">
+        <v>0.40785729999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="11">
+        <v>1.016</v>
+      </c>
+      <c r="D18" s="11">
+        <v>48.126980000000003</v>
+      </c>
+      <c r="E18" s="11">
+        <v>4</v>
+      </c>
+      <c r="F18" s="11">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="G18" s="11">
+        <v>24.6</v>
+      </c>
+      <c r="H18" s="11">
+        <v>18.8</v>
+      </c>
+      <c r="I18" s="11">
+        <v>6.8937080000000001E-3</v>
+      </c>
+      <c r="J18" s="11">
+        <v>1.835056</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0.30508475000000002</v>
+      </c>
+      <c r="L18" s="11">
+        <v>0.43721976000000001</v>
+      </c>
+      <c r="M18" s="11">
+        <v>0.3333333</v>
+      </c>
+      <c r="N18" s="11">
+        <v>0.12610566000000001</v>
+      </c>
+      <c r="O18" s="11">
+        <v>0.9186434</v>
+      </c>
+      <c r="P18" s="11">
+        <v>0.21791045000000001</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>6.51341E-2</v>
+      </c>
+      <c r="R18" s="11">
+        <v>0.37955430000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="11">
+        <v>1.143</v>
+      </c>
+      <c r="D19" s="11">
+        <v>55.122799999999998</v>
+      </c>
+      <c r="E19" s="11">
+        <v>5</v>
+      </c>
+      <c r="F19" s="11">
+        <v>101.42856999999999</v>
+      </c>
+      <c r="G19" s="11">
+        <v>14.57</v>
+      </c>
+      <c r="H19" s="11">
+        <v>22.76</v>
+      </c>
+      <c r="I19" s="11">
+        <v>5.8046229999999997E-2</v>
+      </c>
+      <c r="J19" s="11">
+        <v>2.0061599999999999</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0.38983051000000002</v>
+      </c>
+      <c r="L19" s="11">
+        <v>0.52091989999999999</v>
+      </c>
+      <c r="M19" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N19" s="11">
+        <v>9.6752080000000004E-2</v>
+      </c>
+      <c r="O19" s="11">
+        <v>0.64265649999999996</v>
+      </c>
+      <c r="P19" s="11">
+        <v>6.8208959999999999E-2</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>0.11570881199999999</v>
+      </c>
+      <c r="R19" s="11">
+        <v>0.36362820000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0.99060000000000004</v>
+      </c>
+      <c r="D20" s="11">
+        <v>46.785710000000002</v>
+      </c>
+      <c r="E20" s="11">
+        <v>5</v>
+      </c>
+      <c r="F20" s="11">
+        <v>101.71429000000001</v>
+      </c>
+      <c r="G20" s="11">
+        <v>18</v>
+      </c>
+      <c r="H20" s="11">
+        <v>32.14</v>
+      </c>
+      <c r="I20" s="11">
+        <v>-4.1016760000000003E-3</v>
+      </c>
+      <c r="J20" s="11">
+        <v>2.0073820000000002</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0.28813559</v>
+      </c>
+      <c r="L20" s="11">
+        <v>0.42117238000000001</v>
+      </c>
+      <c r="M20" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N20" s="11">
+        <v>0.18916949</v>
+      </c>
+      <c r="O20" s="11">
+        <v>0.64068599999999998</v>
+      </c>
+      <c r="P20" s="11">
+        <v>0.11940299</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>0.23550446999999999</v>
+      </c>
+      <c r="R20" s="11">
+        <v>0.3582243</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="11">
+        <v>1.1684000000000001</v>
+      </c>
+      <c r="D21" s="11">
+        <v>59.424999999999997</v>
+      </c>
+      <c r="E21" s="11">
+        <v>4</v>
+      </c>
+      <c r="F21" s="11">
+        <v>88.857140000000001</v>
+      </c>
+      <c r="G21" s="11">
+        <v>15.14</v>
+      </c>
+      <c r="H21" s="11">
+        <v>14.17</v>
+      </c>
+      <c r="I21" s="11">
+        <v>6.7591548000000001E-2</v>
+      </c>
+      <c r="J21" s="11">
+        <v>1.9486920000000001</v>
+      </c>
+      <c r="K21" s="11">
+        <v>0.40677965999999999</v>
+      </c>
+      <c r="L21" s="11">
+        <v>0.57239278000000005</v>
+      </c>
+      <c r="M21" s="11">
+        <v>0.3333333</v>
+      </c>
+      <c r="N21" s="11">
+        <v>3.4223770000000001E-2</v>
+      </c>
+      <c r="O21" s="11">
+        <v>0.73535090000000003</v>
+      </c>
+      <c r="P21" s="11">
+        <v>7.6716419999999994E-2</v>
+      </c>
+      <c r="Q21" s="11">
+        <v>6.0025540000000002E-3</v>
+      </c>
+      <c r="R21" s="11">
+        <v>0.35509590000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="D22" s="11">
+        <v>17.142859999999999</v>
+      </c>
+      <c r="E22" s="11">
+        <v>2</v>
+      </c>
+      <c r="F22" s="11">
+        <v>154.57142999999999</v>
+      </c>
+      <c r="G22" s="11">
+        <v>55.285710000000002</v>
+      </c>
+      <c r="H22" s="11">
+        <v>71.7</v>
+      </c>
+      <c r="I22" s="11">
+        <v>-0.118045029</v>
+      </c>
+      <c r="J22" s="11">
+        <v>2.1891289999999999</v>
+      </c>
+      <c r="K22" s="11">
+        <v>0.13559321999999999</v>
+      </c>
+      <c r="L22" s="11">
+        <v>6.6515900000000003E-2</v>
+      </c>
+      <c r="M22" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N22" s="11">
+        <v>0.71486590000000005</v>
+      </c>
+      <c r="O22" s="11">
+        <v>0.34753200000000001</v>
+      </c>
+      <c r="P22" s="11">
+        <v>0.67590618000000002</v>
+      </c>
+      <c r="Q22" s="11">
+        <v>0.74074074099999998</v>
+      </c>
+      <c r="R22" s="11">
+        <v>0.34623320000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="11">
+        <v>1.016</v>
+      </c>
+      <c r="D23" s="11">
+        <v>25</v>
+      </c>
+      <c r="E23" s="11">
+        <v>5</v>
+      </c>
+      <c r="F23" s="11">
+        <v>118</v>
+      </c>
+      <c r="G23" s="11">
+        <v>15.43</v>
+      </c>
+      <c r="H23" s="11">
+        <v>27.95</v>
+      </c>
+      <c r="I23" s="11">
+        <v>6.8937080000000001E-3</v>
+      </c>
+      <c r="J23" s="11">
+        <v>2.071882</v>
+      </c>
+      <c r="K23" s="11">
+        <v>0.30508475000000002</v>
+      </c>
+      <c r="L23" s="11">
+        <v>0.16052122999999999</v>
+      </c>
+      <c r="M23" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N23" s="11">
+        <v>0.14170514000000001</v>
+      </c>
+      <c r="O23" s="11">
+        <v>0.53664900000000004</v>
+      </c>
+      <c r="P23" s="11">
+        <v>8.1044779999999997E-2</v>
+      </c>
+      <c r="Q23" s="11">
+        <v>0.181992337</v>
+      </c>
+      <c r="R23" s="11">
+        <v>0.28495609999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0.83819999999999995</v>
+      </c>
+      <c r="D24" s="11">
+        <v>11.58333</v>
+      </c>
+      <c r="E24" s="11">
+        <v>2</v>
+      </c>
+      <c r="F24" s="11">
+        <v>117.85714</v>
+      </c>
+      <c r="G24" s="11">
+        <v>32.43</v>
+      </c>
+      <c r="H24" s="11">
+        <v>55.28</v>
+      </c>
+      <c r="I24" s="11">
+        <v>-7.6652343999999997E-2</v>
+      </c>
+      <c r="J24" s="11">
+        <v>2.0713560000000002</v>
+      </c>
+      <c r="K24" s="11">
+        <v>0.18644068</v>
+      </c>
+      <c r="L24" s="11">
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N24" s="11">
+        <v>0.45270967000000001</v>
+      </c>
+      <c r="O24" s="11">
+        <v>0.53749749999999996</v>
+      </c>
+      <c r="P24" s="11">
+        <v>0.33477612000000001</v>
+      </c>
+      <c r="Q24" s="11">
+        <v>0.531034483</v>
+      </c>
+      <c r="R24" s="11">
+        <v>0.28347670000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="11">
+        <v>1.0414000000000001</v>
+      </c>
+      <c r="D25" s="11">
+        <v>27.410509999999999</v>
+      </c>
+      <c r="E25" s="11">
+        <v>2</v>
+      </c>
+      <c r="F25" s="11">
+        <v>79.8</v>
+      </c>
+      <c r="G25" s="11">
+        <v>16.7</v>
+      </c>
+      <c r="H25" s="11">
+        <v>25.6</v>
+      </c>
+      <c r="I25" s="11">
+        <v>1.7617573000000001E-2</v>
+      </c>
+      <c r="J25" s="11">
+        <v>1.9020030000000001</v>
+      </c>
+      <c r="K25" s="11">
+        <v>0.32203389999999998</v>
+      </c>
+      <c r="L25" s="11">
+        <v>0.18936128999999999</v>
+      </c>
+      <c r="M25" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N25" s="11">
+        <v>0.13123502000000001</v>
+      </c>
+      <c r="O25" s="11">
+        <v>0.81065989999999999</v>
+      </c>
+      <c r="P25" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="Q25" s="11">
+        <v>0.15197956600000001</v>
+      </c>
+      <c r="R25" s="11">
+        <v>0.28085759999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="D26" s="11">
+        <v>17.585760000000001</v>
+      </c>
+      <c r="E26" s="11">
+        <v>1</v>
+      </c>
+      <c r="F26" s="11">
+        <v>182.85713999999999</v>
+      </c>
+      <c r="G26" s="11">
+        <v>48.428570000000001</v>
+      </c>
+      <c r="H26" s="11">
+        <v>63.4</v>
+      </c>
+      <c r="I26" s="11">
+        <v>-0.118045029</v>
+      </c>
+      <c r="J26" s="11">
+        <v>2.2621120000000001</v>
+      </c>
+      <c r="K26" s="11">
+        <v>0.13559321999999999</v>
+      </c>
+      <c r="L26" s="11">
+        <v>7.1814989999999995E-2</v>
+      </c>
+      <c r="M26" s="11">
+        <v>0</v>
+      </c>
+      <c r="N26" s="11">
+        <v>0.61032286999999996</v>
+      </c>
+      <c r="O26" s="11">
+        <v>0.22981270000000001</v>
+      </c>
+      <c r="P26" s="11">
+        <v>0.57356077000000005</v>
+      </c>
+      <c r="Q26" s="11">
+        <v>0.63473818599999998</v>
+      </c>
+      <c r="R26" s="11">
+        <v>0.27425329999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="11">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="D27" s="11">
+        <v>15.87133</v>
+      </c>
+      <c r="E27" s="11">
+        <v>2</v>
+      </c>
+      <c r="F27" s="11">
+        <v>107.71429000000001</v>
+      </c>
+      <c r="G27" s="11">
+        <v>25.71</v>
+      </c>
+      <c r="H27" s="11">
+        <v>47.88</v>
+      </c>
+      <c r="I27" s="11">
+        <v>-0.19722627500000001</v>
+      </c>
+      <c r="J27" s="11">
+        <v>2.032273</v>
+      </c>
+      <c r="K27" s="11">
+        <v>5.0847459999999997E-2</v>
+      </c>
+      <c r="L27" s="11">
+        <v>5.1303000000000001E-2</v>
+      </c>
+      <c r="M27" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N27" s="11">
+        <v>0.35589056000000002</v>
+      </c>
+      <c r="O27" s="11">
+        <v>0.60053679999999998</v>
+      </c>
+      <c r="P27" s="11">
+        <v>0.23447761</v>
+      </c>
+      <c r="Q27" s="11">
+        <v>0.43652618100000001</v>
+      </c>
+      <c r="R27" s="11">
+        <v>0.24746699999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="11">
+        <v>0.91439999999999999</v>
+      </c>
+      <c r="D28" s="11">
+        <v>37.192999999999998</v>
+      </c>
+      <c r="E28" s="11">
+        <v>2</v>
+      </c>
+      <c r="F28" s="11">
+        <v>122.85714</v>
+      </c>
+      <c r="G28" s="11">
+        <v>17.14</v>
+      </c>
+      <c r="H28" s="11">
+        <v>28.68</v>
+      </c>
+      <c r="I28" s="11">
+        <v>-3.8863782999999999E-2</v>
+      </c>
+      <c r="J28" s="11">
+        <v>2.0893999999999999</v>
+      </c>
+      <c r="K28" s="11">
+        <v>0.23728814000000001</v>
+      </c>
+      <c r="L28" s="11">
+        <v>0.30640212999999999</v>
+      </c>
+      <c r="M28" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N28" s="11">
+        <v>0.15749323000000001</v>
+      </c>
+      <c r="O28" s="11">
+        <v>0.50839219999999996</v>
+      </c>
+      <c r="P28" s="11">
+        <v>0.10656715999999999</v>
+      </c>
+      <c r="Q28" s="11">
+        <v>0.191315453</v>
+      </c>
+      <c r="R28" s="11">
+        <v>0.2435127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0.68579999999999997</v>
+      </c>
+      <c r="D29" s="11">
+        <v>27.081019999999999</v>
+      </c>
+      <c r="E29" s="11">
+        <v>2</v>
+      </c>
+      <c r="F29" s="11">
+        <v>60.9</v>
+      </c>
+      <c r="G29" s="11">
+        <v>10</v>
+      </c>
+      <c r="H29" s="11">
+        <v>13.7</v>
+      </c>
+      <c r="I29" s="11">
+        <v>-0.16380251900000001</v>
+      </c>
+      <c r="J29" s="11">
+        <v>1.7846169999999999</v>
+      </c>
+      <c r="K29" s="11">
+        <v>8.4745760000000003E-2</v>
+      </c>
+      <c r="L29" s="11">
+        <v>0.18541924000000001</v>
+      </c>
+      <c r="M29" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N29" s="11">
+        <v>0</v>
+      </c>
+      <c r="O29" s="11">
+        <v>1</v>
+      </c>
+      <c r="P29" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="11">
+        <v>0</v>
+      </c>
+      <c r="R29" s="11">
+        <v>0.23021269999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="11">
+        <v>0.81279999999999997</v>
+      </c>
+      <c r="D30" s="11">
+        <v>13.53</v>
+      </c>
+      <c r="E30" s="11">
+        <v>1</v>
+      </c>
+      <c r="F30" s="11">
+        <v>253.85713999999999</v>
+      </c>
+      <c r="G30" s="11">
+        <v>40</v>
+      </c>
+      <c r="H30" s="11">
+        <v>62.2</v>
+      </c>
+      <c r="I30" s="11">
+        <v>-9.0016305000000005E-2</v>
+      </c>
+      <c r="J30" s="11">
+        <v>2.4045890000000001</v>
+      </c>
+      <c r="K30" s="11">
+        <v>0.16949153</v>
+      </c>
+      <c r="L30" s="11">
+        <v>2.3290539999999998E-2</v>
+      </c>
+      <c r="M30" s="11">
+        <v>0</v>
+      </c>
+      <c r="N30" s="11">
+        <v>0.55090813999999999</v>
+      </c>
+      <c r="O30" s="11">
+        <v>0</v>
+      </c>
+      <c r="P30" s="11">
+        <v>0.44776118999999998</v>
+      </c>
+      <c r="Q30" s="11">
+        <v>0.61941251600000002</v>
+      </c>
+      <c r="R30" s="11">
+        <v>0.2099926</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="11">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="D31" s="11">
+        <v>16.256150000000002</v>
+      </c>
+      <c r="E31" s="11">
+        <v>2</v>
+      </c>
+      <c r="F31" s="11">
+        <v>102.28570999999999</v>
+      </c>
+      <c r="G31" s="11">
+        <v>16</v>
+      </c>
+      <c r="H31" s="11">
+        <v>29.14</v>
+      </c>
+      <c r="I31" s="11">
+        <v>-0.19722627500000001</v>
+      </c>
+      <c r="J31" s="11">
+        <v>2.0098150000000001</v>
+      </c>
+      <c r="K31" s="11">
+        <v>5.0847459999999997E-2</v>
+      </c>
+      <c r="L31" s="11">
+        <v>5.5907100000000001E-2</v>
+      </c>
+      <c r="M31" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N31" s="11">
+        <v>0.15423298999999999</v>
+      </c>
+      <c r="O31" s="11">
+        <v>0.63676160000000004</v>
+      </c>
+      <c r="P31" s="11">
+        <v>8.9552240000000005E-2</v>
+      </c>
+      <c r="Q31" s="11">
+        <v>0.19719029399999999</v>
+      </c>
+      <c r="R31" s="11">
+        <v>0.19022829999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D50B38-E8D7-DB4C-9637-7546ACA0226F}">
+  <dimension ref="A1:R30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R10" sqref="A10:R20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="8"/>
+      <c r="B1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="11">
+        <v>2.0573999999999999</v>
+      </c>
+      <c r="D2" s="11">
+        <v>95.165220000000005</v>
+      </c>
+      <c r="E2" s="11">
+        <v>5</v>
+      </c>
+      <c r="F2" s="11">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="G2" s="11">
+        <v>59.4</v>
+      </c>
+      <c r="H2" s="11">
+        <v>86.1</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0.31331873500000001</v>
+      </c>
+      <c r="J2" s="11">
+        <v>1.865696</v>
+      </c>
+      <c r="K2" s="11">
+        <v>1</v>
+      </c>
+      <c r="L2" s="11">
+        <v>1</v>
+      </c>
+      <c r="M2" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N2" s="11">
+        <v>0.84988505999999997</v>
+      </c>
+      <c r="O2" s="11">
+        <v>0.86922189999999999</v>
+      </c>
+      <c r="P2" s="11">
+        <v>0.73731343000000005</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>0.92464878699999997</v>
+      </c>
+      <c r="R2" s="11">
+        <v>0.83271030000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1.7272000000000001</v>
+      </c>
+      <c r="D3" s="11">
+        <v>51.416670000000003</v>
+      </c>
+      <c r="E3" s="11">
+        <v>10</v>
+      </c>
+      <c r="F3" s="11">
+        <v>79.2</v>
+      </c>
+      <c r="G3" s="11">
+        <v>67.3</v>
+      </c>
+      <c r="H3" s="11">
+        <v>90</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0.237342629</v>
+      </c>
+      <c r="J3" s="11">
+        <v>1.898725</v>
+      </c>
+      <c r="K3" s="11">
+        <v>0.77966102000000004</v>
+      </c>
+      <c r="L3" s="11">
+        <v>0.47657855999999998</v>
+      </c>
+      <c r="M3" s="11">
+        <v>1</v>
+      </c>
+      <c r="N3" s="11">
+        <v>0.92687235000000001</v>
+      </c>
+      <c r="O3" s="11">
+        <v>0.81594670000000002</v>
+      </c>
+      <c r="P3" s="11">
+        <v>0.85522388000000005</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>0.97445721600000001</v>
+      </c>
+      <c r="R3" s="11">
+        <v>0.79981170000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="11">
+        <v>1.6002000000000001</v>
+      </c>
+      <c r="D4" s="11">
+        <v>41.229050000000001</v>
+      </c>
+      <c r="E4" s="11">
+        <v>10</v>
+      </c>
+      <c r="F4" s="11">
+        <v>79.7</v>
+      </c>
+      <c r="G4" s="11">
+        <v>77</v>
+      </c>
+      <c r="H4" s="11">
+        <v>92</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.20417426599999999</v>
+      </c>
+      <c r="J4" s="11">
+        <v>1.9014580000000001</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0.69491524999999998</v>
+      </c>
+      <c r="L4" s="11">
+        <v>0.35469067999999998</v>
+      </c>
+      <c r="M4" s="11">
+        <v>1</v>
+      </c>
+      <c r="N4" s="11">
+        <v>1</v>
+      </c>
+      <c r="O4" s="11">
+        <v>0.81153819999999999</v>
+      </c>
+      <c r="P4" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>1</v>
+      </c>
+      <c r="R4" s="11">
+        <v>0.77222880000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="11">
+        <v>2.0573999999999999</v>
+      </c>
+      <c r="D5" s="11">
+        <v>85.578950000000006</v>
+      </c>
+      <c r="E5" s="11">
+        <v>8</v>
+      </c>
+      <c r="F5" s="11">
+        <v>148.5</v>
+      </c>
+      <c r="G5" s="11">
+        <v>42.6</v>
+      </c>
+      <c r="H5" s="11">
+        <v>75.8</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0.31331873500000001</v>
+      </c>
+      <c r="J5" s="11">
+        <v>2.171726</v>
+      </c>
+      <c r="K5" s="11">
+        <v>1</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0.88530684000000004</v>
+      </c>
+      <c r="M5" s="11">
+        <v>0.77777779999999996</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0.67076778999999997</v>
+      </c>
+      <c r="O5" s="11">
+        <v>0.3756023</v>
+      </c>
+      <c r="P5" s="11">
+        <v>0.48656716</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>0.79310344799999999</v>
+      </c>
+      <c r="R5" s="11">
+        <v>0.74189090000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1.8288</v>
+      </c>
+      <c r="D6" s="11">
+        <v>62.285710000000002</v>
+      </c>
+      <c r="E6" s="11">
+        <v>10</v>
+      </c>
+      <c r="F6" s="11">
+        <v>128.5</v>
+      </c>
+      <c r="G6" s="11">
+        <v>55.6</v>
+      </c>
+      <c r="H6" s="11">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0.26216621299999998</v>
+      </c>
+      <c r="J6" s="11">
+        <v>2.1089030000000002</v>
+      </c>
+      <c r="K6" s="11">
+        <v>0.84745762999999996</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0.60661925999999999</v>
+      </c>
+      <c r="M6" s="11">
+        <v>1</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0.75818001000000002</v>
+      </c>
+      <c r="O6" s="11">
+        <v>0.47693479999999999</v>
+      </c>
+      <c r="P6" s="11">
+        <v>0.68059700999999995</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>0.80970625799999996</v>
+      </c>
+      <c r="R6" s="11">
+        <v>0.73783829999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1.6002000000000001</v>
+      </c>
+      <c r="D7" s="11">
+        <v>51.095239999999997</v>
+      </c>
+      <c r="E7" s="11">
+        <v>9</v>
+      </c>
+      <c r="F7" s="11">
+        <v>89.857140000000001</v>
+      </c>
+      <c r="G7" s="11">
+        <v>27.86</v>
+      </c>
+      <c r="H7" s="11">
+        <v>34.590000000000003</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.20417426599999999</v>
+      </c>
+      <c r="J7" s="11">
+        <v>1.9535530000000001</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0.69491524999999998</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0.47273288000000002</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0.88888889999999998</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0.26670369999999999</v>
+      </c>
+      <c r="O7" s="11">
+        <v>0.72751140000000003</v>
+      </c>
+      <c r="P7" s="11">
+        <v>0.26656716000000003</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>0.26679438100000002</v>
+      </c>
+      <c r="R7" s="11">
+        <v>0.61015039999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="D8" s="11">
+        <v>62.133330000000001</v>
+      </c>
+      <c r="E8" s="11">
+        <v>6</v>
+      </c>
+      <c r="F8" s="11">
+        <v>90.29</v>
+      </c>
+      <c r="G8" s="11">
+        <v>75.14</v>
+      </c>
+      <c r="H8" s="11">
+        <v>82.78</v>
+      </c>
+      <c r="I8" s="11">
+        <v>-5.1098238999999997E-2</v>
+      </c>
+      <c r="J8" s="11">
+        <v>1.95564</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0.22033897999999999</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0.60479612999999999</v>
+      </c>
+      <c r="M8" s="11">
+        <v>0.55555560000000004</v>
+      </c>
+      <c r="N8" s="11">
+        <v>0.91816231999999998</v>
+      </c>
+      <c r="O8" s="11">
+        <v>0.72414509999999999</v>
+      </c>
+      <c r="P8" s="11">
+        <v>0.97223881000000001</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>0.88224776500000002</v>
+      </c>
+      <c r="R8" s="11">
+        <v>0.60459960000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2.0573999999999999</v>
+      </c>
+      <c r="D9" s="11">
+        <v>50</v>
+      </c>
+      <c r="E9" s="11">
+        <v>6</v>
+      </c>
+      <c r="F9" s="11">
+        <v>115.57143000000001</v>
+      </c>
+      <c r="G9" s="11">
+        <v>21.71</v>
+      </c>
+      <c r="H9" s="11">
+        <v>31.37</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0.31331873500000001</v>
+      </c>
+      <c r="J9" s="11">
+        <v>2.0628500000000001</v>
+      </c>
+      <c r="K9" s="11">
+        <v>1</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0.45962911000000001</v>
+      </c>
+      <c r="M9" s="11">
+        <v>0.55555560000000004</v>
+      </c>
+      <c r="N9" s="11">
+        <v>0.20535903999999999</v>
+      </c>
+      <c r="O9" s="11">
+        <v>0.55121659999999995</v>
+      </c>
+      <c r="P9" s="11">
+        <v>0.17477612000000001</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>0.225670498</v>
+      </c>
+      <c r="R9" s="11">
+        <v>0.55435210000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="11">
+        <v>1.524</v>
+      </c>
+      <c r="D10" s="11">
+        <v>48.083329999999997</v>
+      </c>
+      <c r="E10" s="11">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11">
+        <v>105</v>
+      </c>
+      <c r="G10" s="11">
+        <v>25.29</v>
+      </c>
+      <c r="H10" s="11">
+        <v>46.64</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0.182984967</v>
+      </c>
+      <c r="J10" s="11">
+        <v>2.0211890000000001</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0.64406779999999997</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0.43669750000000002</v>
+      </c>
+      <c r="M10" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N10" s="11">
+        <v>0.34387246999999999</v>
+      </c>
+      <c r="O10" s="11">
+        <v>0.6184151</v>
+      </c>
+      <c r="P10" s="11">
+        <v>0.22820895999999999</v>
+      </c>
+      <c r="Q10" s="11">
+        <v>0.420689655</v>
+      </c>
+      <c r="R10" s="11">
+        <v>0.49749949999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="11">
+        <v>1.1938</v>
+      </c>
+      <c r="D11" s="11">
+        <v>51.27</v>
+      </c>
+      <c r="E11" s="11">
+        <v>5</v>
+      </c>
+      <c r="F11" s="11">
+        <v>79.8</v>
+      </c>
+      <c r="G11" s="11">
+        <v>38.4</v>
+      </c>
+      <c r="H11" s="11">
+        <v>32</v>
+      </c>
+      <c r="I11" s="11">
+        <v>7.6931575000000002E-2</v>
+      </c>
+      <c r="J11" s="11">
+        <v>1.9020030000000001</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0.42372881000000001</v>
+      </c>
+      <c r="L11" s="11">
+        <v>0.47482379000000002</v>
+      </c>
+      <c r="M11" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N11" s="11">
+        <v>0.30960913000000001</v>
+      </c>
+      <c r="O11" s="11">
+        <v>0.81065989999999999</v>
+      </c>
+      <c r="P11" s="11">
+        <v>0.4238806</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>0.23371647500000001</v>
+      </c>
+      <c r="R11" s="11">
+        <v>0.49265320000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1.6002000000000001</v>
+      </c>
+      <c r="D12" s="11">
+        <v>54.256189999999997</v>
+      </c>
+      <c r="E12" s="11">
+        <v>5</v>
+      </c>
+      <c r="F12" s="11">
+        <v>105.8</v>
+      </c>
+      <c r="G12" s="11">
+        <v>26.2</v>
+      </c>
+      <c r="H12" s="11">
+        <v>26.6</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0.20417426599999999</v>
+      </c>
+      <c r="J12" s="11">
+        <v>2.024486</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0.69491524999999998</v>
+      </c>
+      <c r="L12" s="11">
+        <v>0.51055156000000002</v>
+      </c>
+      <c r="M12" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N12" s="11">
+        <v>0.19549691</v>
+      </c>
+      <c r="O12" s="11">
+        <v>0.61309809999999998</v>
+      </c>
+      <c r="P12" s="11">
+        <v>0.24179104000000001</v>
+      </c>
+      <c r="Q12" s="11">
+        <v>0.164750958</v>
+      </c>
+      <c r="R12" s="11">
+        <v>0.49170130000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="11">
+        <v>1.2192000000000001</v>
+      </c>
+      <c r="D13" s="11">
+        <v>46.307690000000001</v>
+      </c>
+      <c r="E13" s="11">
+        <v>4</v>
+      </c>
+      <c r="F13" s="11">
+        <v>97.285709999999995</v>
+      </c>
+      <c r="G13" s="11">
+        <v>22.86</v>
+      </c>
+      <c r="H13" s="11">
+        <v>44.54</v>
+      </c>
+      <c r="I13" s="11">
+        <v>8.6074953999999995E-2</v>
+      </c>
+      <c r="J13" s="11">
+        <v>1.988049</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0.44067796999999997</v>
+      </c>
+      <c r="L13" s="11">
+        <v>0.41545316999999998</v>
+      </c>
+      <c r="M13" s="11">
+        <v>0.3333333</v>
+      </c>
+      <c r="N13" s="11">
+        <v>0.31328165000000002</v>
+      </c>
+      <c r="O13" s="11">
+        <v>0.67186950000000001</v>
+      </c>
+      <c r="P13" s="11">
+        <v>0.19194030000000001</v>
+      </c>
+      <c r="Q13" s="11">
+        <v>0.39386973199999997</v>
+      </c>
+      <c r="R13" s="11">
+        <v>0.43492310000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="D14" s="11">
+        <v>51.191670000000002</v>
+      </c>
+      <c r="E14" s="11">
+        <v>5</v>
+      </c>
+      <c r="F14" s="11">
+        <v>113.2</v>
+      </c>
+      <c r="G14" s="11">
+        <v>42.4</v>
+      </c>
+      <c r="H14" s="11">
+        <v>45.7</v>
+      </c>
+      <c r="I14" s="11">
+        <v>-5.1098238999999997E-2</v>
+      </c>
+      <c r="J14" s="11">
+        <v>2.0538460000000001</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0.22033897999999999</v>
+      </c>
+      <c r="L14" s="11">
+        <v>0.47388659</v>
+      </c>
+      <c r="M14" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0.43857542999999999</v>
+      </c>
+      <c r="O14" s="11">
+        <v>0.56573989999999996</v>
+      </c>
+      <c r="P14" s="11">
+        <v>0.48358209000000002</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>0.40868454700000001</v>
+      </c>
+      <c r="R14" s="11">
+        <v>0.42859710000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="11">
+        <v>1.016</v>
+      </c>
+      <c r="D15" s="11">
+        <v>48.126980000000003</v>
+      </c>
+      <c r="E15" s="11">
+        <v>4</v>
+      </c>
+      <c r="F15" s="11">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="G15" s="11">
+        <v>24.6</v>
+      </c>
+      <c r="H15" s="11">
+        <v>18.8</v>
+      </c>
+      <c r="I15" s="11">
+        <v>6.8937080000000001E-3</v>
+      </c>
+      <c r="J15" s="11">
+        <v>1.835056</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0.30508475000000002</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0.43721976000000001</v>
+      </c>
+      <c r="M15" s="11">
+        <v>0.3333333</v>
+      </c>
+      <c r="N15" s="11">
+        <v>0.12610566000000001</v>
+      </c>
+      <c r="O15" s="11">
+        <v>0.9186434</v>
+      </c>
+      <c r="P15" s="11">
+        <v>0.21791045000000001</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>6.51341E-2</v>
+      </c>
+      <c r="R15" s="11">
+        <v>0.42407739999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="11">
+        <v>1.143</v>
+      </c>
+      <c r="D16" s="11">
+        <v>55.122799999999998</v>
+      </c>
+      <c r="E16" s="11">
+        <v>5</v>
+      </c>
+      <c r="F16" s="11">
+        <v>101.42856999999999</v>
+      </c>
+      <c r="G16" s="11">
+        <v>14.57</v>
+      </c>
+      <c r="H16" s="11">
+        <v>22.76</v>
+      </c>
+      <c r="I16" s="11">
+        <v>5.8046229999999997E-2</v>
+      </c>
+      <c r="J16" s="11">
+        <v>2.0061599999999999</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0.38983051000000002</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0.52091989999999999</v>
+      </c>
+      <c r="M16" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N16" s="11">
+        <v>9.6752080000000004E-2</v>
+      </c>
+      <c r="O16" s="11">
+        <v>0.64265649999999996</v>
+      </c>
+      <c r="P16" s="11">
+        <v>6.8208959999999999E-2</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>0.11570881199999999</v>
+      </c>
+      <c r="R16" s="11">
+        <v>0.41892069999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="11">
+        <v>1.1684000000000001</v>
+      </c>
+      <c r="D17" s="11">
+        <v>59.424999999999997</v>
+      </c>
+      <c r="E17" s="11">
+        <v>4</v>
+      </c>
+      <c r="F17" s="11">
+        <v>88.857140000000001</v>
+      </c>
+      <c r="G17" s="11">
+        <v>15.14</v>
+      </c>
+      <c r="H17" s="11">
+        <v>14.17</v>
+      </c>
+      <c r="I17" s="11">
+        <v>6.7591548000000001E-2</v>
+      </c>
+      <c r="J17" s="11">
+        <v>1.9486920000000001</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0.40677965999999999</v>
+      </c>
+      <c r="L17" s="11">
+        <v>0.57239278000000005</v>
+      </c>
+      <c r="M17" s="11">
+        <v>0.3333333</v>
+      </c>
+      <c r="N17" s="11">
+        <v>3.4223770000000001E-2</v>
+      </c>
+      <c r="O17" s="11">
+        <v>0.73535090000000003</v>
+      </c>
+      <c r="P17" s="11">
+        <v>7.6716419999999994E-2</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>6.0025540000000002E-3</v>
+      </c>
+      <c r="R17" s="11">
+        <v>0.41641610000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="11">
+        <v>0.99060000000000004</v>
+      </c>
+      <c r="D18" s="11">
+        <v>46.785710000000002</v>
+      </c>
+      <c r="E18" s="11">
+        <v>5</v>
+      </c>
+      <c r="F18" s="11">
+        <v>101.71429000000001</v>
+      </c>
+      <c r="G18" s="11">
+        <v>18</v>
+      </c>
+      <c r="H18" s="11">
+        <v>32.14</v>
+      </c>
+      <c r="I18" s="11">
+        <v>-4.1016760000000003E-3</v>
+      </c>
+      <c r="J18" s="11">
+        <v>2.0073820000000002</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0.28813559</v>
+      </c>
+      <c r="L18" s="11">
+        <v>0.42117238000000001</v>
+      </c>
+      <c r="M18" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N18" s="11">
+        <v>0.18916949</v>
+      </c>
+      <c r="O18" s="11">
+        <v>0.64068599999999998</v>
+      </c>
+      <c r="P18" s="11">
+        <v>0.11940299</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>0.23550446999999999</v>
+      </c>
+      <c r="R18" s="11">
+        <v>0.39672160000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="11">
+        <v>0.71120000000000005</v>
+      </c>
+      <c r="D19" s="11">
+        <v>26.05556</v>
+      </c>
+      <c r="E19" s="11">
+        <v>3</v>
+      </c>
+      <c r="F19" s="11">
+        <v>101.18095</v>
+      </c>
+      <c r="G19" s="11">
+        <v>58.142859999999999</v>
+      </c>
+      <c r="H19" s="11">
+        <v>79.866669999999999</v>
+      </c>
+      <c r="I19" s="11">
+        <v>-0.14800825200000001</v>
+      </c>
+      <c r="J19" s="11">
+        <v>2.005099</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0.10169491999999999</v>
+      </c>
+      <c r="L19" s="11">
+        <v>0.17315024000000001</v>
+      </c>
+      <c r="M19" s="11">
+        <v>0.22222220000000001</v>
+      </c>
+      <c r="N19" s="11">
+        <v>0.79455938000000004</v>
+      </c>
+      <c r="O19" s="11">
+        <v>0.64436870000000002</v>
+      </c>
+      <c r="P19" s="11">
+        <v>0.71855011000000002</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>0.84504044300000003</v>
+      </c>
+      <c r="R19" s="11">
+        <v>0.38719910000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0.55879999999999996</v>
+      </c>
+      <c r="D20" s="11">
+        <v>35.4375</v>
+      </c>
+      <c r="E20" s="11">
+        <v>6</v>
+      </c>
+      <c r="F20" s="11">
+        <v>134.14286000000001</v>
+      </c>
+      <c r="G20" s="11">
+        <v>48</v>
+      </c>
+      <c r="H20" s="11">
+        <v>65.69</v>
+      </c>
+      <c r="I20" s="11">
+        <v>-0.25274360299999998</v>
+      </c>
+      <c r="J20" s="11">
+        <v>2.1275680000000001</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0</v>
+      </c>
+      <c r="L20" s="11">
+        <v>0.28539877000000002</v>
+      </c>
+      <c r="M20" s="11">
+        <v>0.55555560000000004</v>
+      </c>
+      <c r="N20" s="11">
+        <v>0.62534455</v>
+      </c>
+      <c r="O20" s="11">
+        <v>0.44682949999999999</v>
+      </c>
+      <c r="P20" s="11">
+        <v>0.56716418000000002</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>0.66398467400000005</v>
+      </c>
+      <c r="R20" s="11">
+        <v>0.38262570000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="11">
+        <v>1.016</v>
+      </c>
+      <c r="D21" s="11">
+        <v>25</v>
+      </c>
+      <c r="E21" s="11">
+        <v>5</v>
+      </c>
+      <c r="F21" s="11">
+        <v>118</v>
+      </c>
+      <c r="G21" s="11">
+        <v>15.43</v>
+      </c>
+      <c r="H21" s="11">
+        <v>27.95</v>
+      </c>
+      <c r="I21" s="11">
+        <v>6.8937080000000001E-3</v>
+      </c>
+      <c r="J21" s="11">
+        <v>2.071882</v>
+      </c>
+      <c r="K21" s="11">
+        <v>0.30508475000000002</v>
+      </c>
+      <c r="L21" s="11">
+        <v>0.16052122999999999</v>
+      </c>
+      <c r="M21" s="11">
+        <v>0.44444440000000002</v>
+      </c>
+      <c r="N21" s="11">
+        <v>0.14170514000000001</v>
+      </c>
+      <c r="O21" s="11">
+        <v>0.53664900000000004</v>
+      </c>
+      <c r="P21" s="11">
+        <v>8.1044779999999997E-2</v>
+      </c>
+      <c r="Q21" s="11">
+        <v>0.181992337</v>
+      </c>
+      <c r="R21" s="11">
+        <v>0.31768089999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="11">
+        <v>1.0414000000000001</v>
+      </c>
+      <c r="D22" s="11">
+        <v>27.410509999999999</v>
+      </c>
+      <c r="E22" s="11">
+        <v>2</v>
+      </c>
+      <c r="F22" s="11">
+        <v>79.8</v>
+      </c>
+      <c r="G22" s="11">
+        <v>16.7</v>
+      </c>
+      <c r="H22" s="11">
+        <v>25.6</v>
+      </c>
+      <c r="I22" s="11">
+        <v>1.7617573000000001E-2</v>
+      </c>
+      <c r="J22" s="11">
+        <v>1.9020030000000001</v>
+      </c>
+      <c r="K22" s="11">
+        <v>0.32203389999999998</v>
+      </c>
+      <c r="L22" s="11">
+        <v>0.18936128999999999</v>
+      </c>
+      <c r="M22" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N22" s="11">
+        <v>0.13123502000000001</v>
+      </c>
+      <c r="O22" s="11">
+        <v>0.81065989999999999</v>
+      </c>
+      <c r="P22" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="Q22" s="11">
+        <v>0.15197956600000001</v>
+      </c>
+      <c r="R22" s="11">
+        <v>0.3128802</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0.68579999999999997</v>
+      </c>
+      <c r="D23" s="11">
+        <v>27.081019999999999</v>
+      </c>
+      <c r="E23" s="11">
+        <v>2</v>
+      </c>
+      <c r="F23" s="11">
+        <v>60.9</v>
+      </c>
+      <c r="G23" s="11">
+        <v>10</v>
+      </c>
+      <c r="H23" s="11">
+        <v>13.7</v>
+      </c>
+      <c r="I23" s="11">
+        <v>-0.16380251900000001</v>
+      </c>
+      <c r="J23" s="11">
+        <v>1.7846169999999999</v>
+      </c>
+      <c r="K23" s="11">
+        <v>8.4745760000000003E-2</v>
+      </c>
+      <c r="L23" s="11">
+        <v>0.18541924000000001</v>
+      </c>
+      <c r="M23" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N23" s="11">
+        <v>0</v>
+      </c>
+      <c r="O23" s="11">
+        <v>1</v>
+      </c>
+      <c r="P23" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="11">
+        <v>0</v>
+      </c>
+      <c r="R23" s="11">
+        <v>0.27625519999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="D24" s="11">
+        <v>17.142859999999999</v>
+      </c>
+      <c r="E24" s="11">
+        <v>2</v>
+      </c>
+      <c r="F24" s="11">
+        <v>154.57142999999999</v>
+      </c>
+      <c r="G24" s="11">
+        <v>55.285710000000002</v>
+      </c>
+      <c r="H24" s="11">
+        <v>71.7</v>
+      </c>
+      <c r="I24" s="11">
+        <v>-0.118045029</v>
+      </c>
+      <c r="J24" s="11">
+        <v>2.1891289999999999</v>
+      </c>
+      <c r="K24" s="11">
+        <v>0.13559321999999999</v>
+      </c>
+      <c r="L24" s="11">
+        <v>6.6515900000000003E-2</v>
+      </c>
+      <c r="M24" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N24" s="11">
+        <v>0.71486590000000005</v>
+      </c>
+      <c r="O24" s="11">
+        <v>0.34753200000000001</v>
+      </c>
+      <c r="P24" s="11">
+        <v>0.67590618000000002</v>
+      </c>
+      <c r="Q24" s="11">
+        <v>0.74074074099999998</v>
+      </c>
+      <c r="R24" s="11">
+        <v>0.27512360000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="11">
+        <v>0.91439999999999999</v>
+      </c>
+      <c r="D25" s="11">
+        <v>37.192999999999998</v>
+      </c>
+      <c r="E25" s="11">
+        <v>2</v>
+      </c>
+      <c r="F25" s="11">
+        <v>122.85714</v>
+      </c>
+      <c r="G25" s="11">
+        <v>17.14</v>
+      </c>
+      <c r="H25" s="11">
+        <v>28.68</v>
+      </c>
+      <c r="I25" s="11">
+        <v>-3.8863782999999999E-2</v>
+      </c>
+      <c r="J25" s="11">
+        <v>2.0893999999999999</v>
+      </c>
+      <c r="K25" s="11">
+        <v>0.23728814000000001</v>
+      </c>
+      <c r="L25" s="11">
+        <v>0.30640212999999999</v>
+      </c>
+      <c r="M25" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N25" s="11">
+        <v>0.15749323000000001</v>
+      </c>
+      <c r="O25" s="11">
+        <v>0.50839219999999996</v>
+      </c>
+      <c r="P25" s="11">
+        <v>0.10656715999999999</v>
+      </c>
+      <c r="Q25" s="11">
+        <v>0.191315453</v>
+      </c>
+      <c r="R25" s="11">
+        <v>0.26413740000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0.83819999999999995</v>
+      </c>
+      <c r="D26" s="11">
+        <v>11.58333</v>
+      </c>
+      <c r="E26" s="11">
+        <v>2</v>
+      </c>
+      <c r="F26" s="11">
+        <v>117.85714</v>
+      </c>
+      <c r="G26" s="11">
+        <v>32.43</v>
+      </c>
+      <c r="H26" s="11">
+        <v>55.28</v>
+      </c>
+      <c r="I26" s="11">
+        <v>-7.6652343999999997E-2</v>
+      </c>
+      <c r="J26" s="11">
+        <v>2.0713560000000002</v>
+      </c>
+      <c r="K26" s="11">
+        <v>0.18644068</v>
+      </c>
+      <c r="L26" s="11">
+        <v>0</v>
+      </c>
+      <c r="M26" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N26" s="11">
+        <v>0.45270967000000001</v>
+      </c>
+      <c r="O26" s="11">
+        <v>0.53749749999999996</v>
+      </c>
+      <c r="P26" s="11">
+        <v>0.33477612000000001</v>
+      </c>
+      <c r="Q26" s="11">
+        <v>0.531034483</v>
+      </c>
+      <c r="R26" s="11">
+        <v>0.2575518</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="11">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="D27" s="11">
+        <v>15.87133</v>
+      </c>
+      <c r="E27" s="11">
+        <v>2</v>
+      </c>
+      <c r="F27" s="11">
+        <v>107.71429000000001</v>
+      </c>
+      <c r="G27" s="11">
+        <v>25.71</v>
+      </c>
+      <c r="H27" s="11">
+        <v>47.88</v>
+      </c>
+      <c r="I27" s="11">
+        <v>-0.19722627500000001</v>
+      </c>
+      <c r="J27" s="11">
+        <v>2.032273</v>
+      </c>
+      <c r="K27" s="11">
+        <v>5.0847459999999997E-2</v>
+      </c>
+      <c r="L27" s="11">
+        <v>5.1303000000000001E-2</v>
+      </c>
+      <c r="M27" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N27" s="11">
+        <v>0.35589056000000002</v>
+      </c>
+      <c r="O27" s="11">
+        <v>0.60053679999999998</v>
+      </c>
+      <c r="P27" s="11">
+        <v>0.23447761</v>
+      </c>
+      <c r="Q27" s="11">
+        <v>0.43652618100000001</v>
+      </c>
+      <c r="R27" s="11">
+        <v>0.2339378</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="11">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="D28" s="11">
+        <v>17.585760000000001</v>
+      </c>
+      <c r="E28" s="11">
+        <v>1</v>
+      </c>
+      <c r="F28" s="11">
+        <v>182.85713999999999</v>
+      </c>
+      <c r="G28" s="11">
+        <v>48.428570000000001</v>
+      </c>
+      <c r="H28" s="11">
+        <v>63.4</v>
+      </c>
+      <c r="I28" s="11">
+        <v>-0.118045029</v>
+      </c>
+      <c r="J28" s="11">
+        <v>2.2621120000000001</v>
+      </c>
+      <c r="K28" s="11">
+        <v>0.13559321999999999</v>
+      </c>
+      <c r="L28" s="11">
+        <v>7.1814989999999995E-2</v>
+      </c>
+      <c r="M28" s="11">
+        <v>0</v>
+      </c>
+      <c r="N28" s="11">
+        <v>0.61032286999999996</v>
+      </c>
+      <c r="O28" s="11">
+        <v>0.22981270000000001</v>
+      </c>
+      <c r="P28" s="11">
+        <v>0.57356077000000005</v>
+      </c>
+      <c r="Q28" s="11">
+        <v>0.63473818599999998</v>
+      </c>
+      <c r="R28" s="11">
+        <v>0.2095088</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="D29" s="11">
+        <v>16.256150000000002</v>
+      </c>
+      <c r="E29" s="11">
+        <v>2</v>
+      </c>
+      <c r="F29" s="11">
+        <v>102.28570999999999</v>
+      </c>
+      <c r="G29" s="11">
+        <v>16</v>
+      </c>
+      <c r="H29" s="11">
+        <v>29.14</v>
+      </c>
+      <c r="I29" s="11">
+        <v>-0.19722627500000001</v>
+      </c>
+      <c r="J29" s="11">
+        <v>2.0098150000000001</v>
+      </c>
+      <c r="K29" s="11">
+        <v>5.0847459999999997E-2</v>
+      </c>
+      <c r="L29" s="11">
+        <v>5.5907100000000001E-2</v>
+      </c>
+      <c r="M29" s="11">
+        <v>0.1111111</v>
+      </c>
+      <c r="N29" s="11">
+        <v>0.15423298999999999</v>
+      </c>
+      <c r="O29" s="11">
+        <v>0.63676160000000004</v>
+      </c>
+      <c r="P29" s="11">
+        <v>8.9552240000000005E-2</v>
+      </c>
+      <c r="Q29" s="11">
+        <v>0.19719029399999999</v>
+      </c>
+      <c r="R29" s="11">
+        <v>0.20177200000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="11">
+        <v>0.81279999999999997</v>
+      </c>
+      <c r="D30" s="11">
+        <v>13.53</v>
+      </c>
+      <c r="E30" s="11">
+        <v>1</v>
+      </c>
+      <c r="F30" s="11">
+        <v>253.85713999999999</v>
+      </c>
+      <c r="G30" s="11">
+        <v>40</v>
+      </c>
+      <c r="H30" s="11">
+        <v>62.2</v>
+      </c>
+      <c r="I30" s="11">
+        <v>-9.0016305000000005E-2</v>
+      </c>
+      <c r="J30" s="11">
+        <v>2.4045890000000001</v>
+      </c>
+      <c r="K30" s="11">
+        <v>0.16949153</v>
+      </c>
+      <c r="L30" s="11">
+        <v>2.3290539999999998E-2</v>
+      </c>
+      <c r="M30" s="11">
+        <v>0</v>
+      </c>
+      <c r="N30" s="11">
+        <v>0.55090813999999999</v>
+      </c>
+      <c r="O30" s="11">
+        <v>0</v>
+      </c>
+      <c r="P30" s="11">
+        <v>0.44776118999999998</v>
+      </c>
+      <c r="Q30" s="11">
+        <v>0.61941251600000002</v>
+      </c>
+      <c r="R30" s="11">
+        <v>0.14873800000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>